<commit_message>
Update 6/24 3rd game
</commit_message>
<xml_diff>
--- a/input/world_cup_2018_final.xlsx
+++ b/input/world_cup_2018_final.xlsx
@@ -9316,90 +9316,6 @@
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -9478,6 +9394,90 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -29896,8 +29896,8 @@
   </sheetPr>
   <dimension ref="A1:BT97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -29952,25 +29952,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:72" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="136" t="str">
+      <c r="A1" s="115" t="str">
         <f>INDEX(T,2,lang)</f>
         <v>2018 World Cup Final Tournament Schedule</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
-      <c r="J1" s="136"/>
-      <c r="K1" s="136"/>
-      <c r="L1" s="136"/>
-      <c r="M1" s="136"/>
-      <c r="N1" s="136"/>
-      <c r="O1" s="136"/>
-      <c r="P1" s="136"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
       <c r="S1" s="58"/>
       <c r="T1" s="58"/>
       <c r="U1" s="58"/>
@@ -30033,11 +30033,11 @@
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
-      <c r="O3" s="137" t="str">
+      <c r="O3" s="116" t="str">
         <f>"Language: " &amp; Settings!C4</f>
         <v>Language: English</v>
       </c>
-      <c r="P3" s="137"/>
+      <c r="P3" s="116"/>
       <c r="S3" s="58"/>
       <c r="T3" s="58"/>
       <c r="U3" s="58"/>
@@ -30063,43 +30063,43 @@
     </row>
     <row r="4" spans="1:72" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="138" t="str">
+      <c r="A5" s="117" t="str">
         <f>INDEX(T,3,lang)</f>
         <v>Group Stage</v>
       </c>
-      <c r="B5" s="139"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="140"/>
-      <c r="J5" s="144" t="s">
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="119"/>
+      <c r="J5" s="123" t="s">
         <v>2174</v>
       </c>
-      <c r="K5" s="145"/>
-      <c r="L5" s="145"/>
-      <c r="M5" s="145"/>
-      <c r="N5" s="145"/>
-      <c r="O5" s="145"/>
-      <c r="P5" s="146"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="124"/>
+      <c r="M5" s="124"/>
+      <c r="N5" s="124"/>
+      <c r="O5" s="124"/>
+      <c r="P5" s="125"/>
     </row>
     <row r="6" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="141"/>
-      <c r="B6" s="142"/>
-      <c r="C6" s="142"/>
-      <c r="D6" s="142"/>
-      <c r="E6" s="142"/>
-      <c r="F6" s="142"/>
-      <c r="G6" s="142"/>
-      <c r="H6" s="143"/>
-      <c r="J6" s="147"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="148"/>
-      <c r="M6" s="148"/>
-      <c r="N6" s="148"/>
-      <c r="O6" s="148"/>
-      <c r="P6" s="149"/>
+      <c r="A6" s="120"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="122"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="127"/>
+      <c r="N6" s="127"/>
+      <c r="O6" s="127"/>
+      <c r="P6" s="128"/>
       <c r="R6" s="58" t="s">
         <v>2175</v>
       </c>
@@ -30163,34 +30163,34 @@
       <c r="AT6" s="62" t="s">
         <v>2182</v>
       </c>
-      <c r="AY6" s="130" t="str">
+      <c r="AY6" s="109" t="str">
         <f>INDEX(T,4,lang)</f>
         <v>Round of 16</v>
       </c>
-      <c r="AZ6" s="131"/>
-      <c r="BA6" s="131"/>
-      <c r="BB6" s="132"/>
-      <c r="BE6" s="130" t="str">
+      <c r="AZ6" s="110"/>
+      <c r="BA6" s="110"/>
+      <c r="BB6" s="111"/>
+      <c r="BE6" s="109" t="str">
         <f>INDEX(T,5,lang)</f>
         <v>Quarterfinals</v>
       </c>
-      <c r="BF6" s="131"/>
-      <c r="BG6" s="131"/>
-      <c r="BH6" s="132"/>
-      <c r="BK6" s="130" t="str">
+      <c r="BF6" s="110"/>
+      <c r="BG6" s="110"/>
+      <c r="BH6" s="111"/>
+      <c r="BK6" s="109" t="str">
         <f>INDEX(T,6,lang)</f>
         <v>Semi-Finals</v>
       </c>
-      <c r="BL6" s="131"/>
-      <c r="BM6" s="131"/>
-      <c r="BN6" s="132"/>
-      <c r="BQ6" s="130" t="str">
+      <c r="BL6" s="110"/>
+      <c r="BM6" s="110"/>
+      <c r="BN6" s="111"/>
+      <c r="BQ6" s="109" t="str">
         <f>INDEX(T,8,lang)</f>
         <v>Final</v>
       </c>
-      <c r="BR6" s="131"/>
-      <c r="BS6" s="131"/>
-      <c r="BT6" s="132"/>
+      <c r="BR6" s="110"/>
+      <c r="BS6" s="110"/>
+      <c r="BT6" s="111"/>
     </row>
     <row r="7" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
@@ -30254,22 +30254,22 @@
         <f>IF(OR(F7="",G7=""),"",IF(F7&gt;G7,1,IF(F7&lt;G7,-1,0)))</f>
         <v>1</v>
       </c>
-      <c r="AY7" s="133"/>
-      <c r="AZ7" s="134"/>
-      <c r="BA7" s="134"/>
-      <c r="BB7" s="135"/>
-      <c r="BE7" s="133"/>
-      <c r="BF7" s="134"/>
-      <c r="BG7" s="134"/>
-      <c r="BH7" s="135"/>
-      <c r="BK7" s="133"/>
-      <c r="BL7" s="134"/>
-      <c r="BM7" s="134"/>
-      <c r="BN7" s="135"/>
-      <c r="BQ7" s="133"/>
-      <c r="BR7" s="134"/>
-      <c r="BS7" s="134"/>
-      <c r="BT7" s="135"/>
+      <c r="AY7" s="112"/>
+      <c r="AZ7" s="113"/>
+      <c r="BA7" s="113"/>
+      <c r="BB7" s="114"/>
+      <c r="BE7" s="112"/>
+      <c r="BF7" s="113"/>
+      <c r="BG7" s="113"/>
+      <c r="BH7" s="114"/>
+      <c r="BK7" s="112"/>
+      <c r="BL7" s="113"/>
+      <c r="BM7" s="113"/>
+      <c r="BN7" s="114"/>
+      <c r="BQ7" s="112"/>
+      <c r="BR7" s="113"/>
+      <c r="BS7" s="113"/>
+      <c r="BT7" s="114"/>
     </row>
     <row r="8" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
@@ -30815,7 +30815,7 @@
         <f>AR10-AS10</f>
         <v>0</v>
       </c>
-      <c r="AY10" s="118">
+      <c r="AY10" s="129">
         <v>49</v>
       </c>
       <c r="AZ10" s="28" t="str">
@@ -31009,7 +31009,7 @@
         <f>AR11-AS11</f>
         <v>0</v>
       </c>
-      <c r="AY11" s="119"/>
+      <c r="AY11" s="130"/>
       <c r="AZ11" s="31" t="str">
         <f>AO15</f>
         <v>2B</v>
@@ -31190,7 +31190,7 @@
       <c r="BB12" s="25"/>
       <c r="BC12" s="36"/>
       <c r="BD12" s="25"/>
-      <c r="BE12" s="118">
+      <c r="BE12" s="129">
         <v>57</v>
       </c>
       <c r="BF12" s="28" t="str">
@@ -31298,7 +31298,7 @@
       <c r="BB13" s="35"/>
       <c r="BC13" s="36"/>
       <c r="BD13" s="39"/>
-      <c r="BE13" s="119"/>
+      <c r="BE13" s="130"/>
       <c r="BF13" s="31" t="str">
         <f>T59</f>
         <v>W50</v>
@@ -31488,7 +31488,7 @@
         <f>AR14-AS14</f>
         <v>0</v>
       </c>
-      <c r="AY14" s="118">
+      <c r="AY14" s="129">
         <v>50</v>
       </c>
       <c r="AZ14" s="28" t="str">
@@ -31686,7 +31686,7 @@
         <f>AR15-AS15</f>
         <v>0</v>
       </c>
-      <c r="AY15" s="119"/>
+      <c r="AY15" s="130"/>
       <c r="AZ15" s="31" t="str">
         <f>AO27</f>
         <v>2D</v>
@@ -31893,7 +31893,7 @@
       <c r="BH16" s="25"/>
       <c r="BI16" s="36"/>
       <c r="BJ16" s="25"/>
-      <c r="BK16" s="118">
+      <c r="BK16" s="129">
         <v>61</v>
       </c>
       <c r="BL16" s="28" t="str">
@@ -32090,7 +32090,7 @@
       <c r="BH17" s="25"/>
       <c r="BI17" s="36"/>
       <c r="BJ17" s="39"/>
-      <c r="BK17" s="119"/>
+      <c r="BK17" s="130"/>
       <c r="BL17" s="31" t="str">
         <f>T70</f>
         <v>W58</v>
@@ -32250,7 +32250,7 @@
         <f>MAX(AT14:AT17)-MIN(AT14:AT17)+1</f>
         <v>1</v>
       </c>
-      <c r="AY18" s="118">
+      <c r="AY18" s="129">
         <v>53</v>
       </c>
       <c r="AZ18" s="28" t="str">
@@ -32355,7 +32355,7 @@
         <f>MIN(AI14:AI17)</f>
         <v>-2</v>
       </c>
-      <c r="AY19" s="119"/>
+      <c r="AY19" s="130"/>
       <c r="AZ19" s="31" t="str">
         <f>AO39</f>
         <v>2F</v>
@@ -32560,7 +32560,7 @@
       <c r="BB20" s="25"/>
       <c r="BC20" s="36"/>
       <c r="BD20" s="25"/>
-      <c r="BE20" s="118">
+      <c r="BE20" s="129">
         <v>58</v>
       </c>
       <c r="BF20" s="28" t="str">
@@ -32761,7 +32761,7 @@
       <c r="BB21" s="35"/>
       <c r="BC21" s="36"/>
       <c r="BD21" s="39"/>
-      <c r="BE21" s="119"/>
+      <c r="BE21" s="130"/>
       <c r="BF21" s="31" t="str">
         <f>T63</f>
         <v>W54</v>
@@ -32947,7 +32947,7 @@
         <f>AR22-AS22</f>
         <v>0</v>
       </c>
-      <c r="AY22" s="118">
+      <c r="AY22" s="129">
         <v>54</v>
       </c>
       <c r="AZ22" s="28" t="str">
@@ -33144,7 +33144,7 @@
         <f>AR23-AS23</f>
         <v>0</v>
       </c>
-      <c r="AY23" s="119"/>
+      <c r="AY23" s="130"/>
       <c r="AZ23" s="31" t="str">
         <f>AO51</f>
         <v>2H</v>
@@ -33165,7 +33165,7 @@
       <c r="BN23" s="25"/>
       <c r="BO23" s="36"/>
       <c r="BP23" s="25"/>
-      <c r="BQ23" s="118">
+      <c r="BQ23" s="129">
         <v>64</v>
       </c>
       <c r="BR23" s="28" t="str">
@@ -33338,7 +33338,7 @@
       <c r="BN24" s="25"/>
       <c r="BO24" s="36"/>
       <c r="BP24" s="39"/>
-      <c r="BQ24" s="119"/>
+      <c r="BQ24" s="130"/>
       <c r="BR24" s="31" t="str">
         <f>T77</f>
         <v>W62</v>
@@ -33619,7 +33619,7 @@
         <f>AR26-AS26</f>
         <v>0</v>
       </c>
-      <c r="AY26" s="118">
+      <c r="AY26" s="129">
         <v>51</v>
       </c>
       <c r="AZ26" s="28" t="str">
@@ -33817,7 +33817,7 @@
         <f>AR27-AS27</f>
         <v>0</v>
       </c>
-      <c r="AY27" s="119"/>
+      <c r="AY27" s="130"/>
       <c r="AZ27" s="31" t="str">
         <f>AO9</f>
         <v>2A</v>
@@ -34018,7 +34018,7 @@
       <c r="BB28" s="25"/>
       <c r="BC28" s="36"/>
       <c r="BD28" s="25"/>
-      <c r="BE28" s="118">
+      <c r="BE28" s="129">
         <v>59</v>
       </c>
       <c r="BF28" s="28" t="str">
@@ -34215,7 +34215,7 @@
       <c r="BB29" s="35"/>
       <c r="BC29" s="36"/>
       <c r="BD29" s="39"/>
-      <c r="BE29" s="119"/>
+      <c r="BE29" s="130"/>
       <c r="BF29" s="31" t="str">
         <f>T61</f>
         <v>W52</v>
@@ -34381,7 +34381,7 @@
         <f>MAX(AT26:AT29)-MIN(AT26:AT29)+1</f>
         <v>1</v>
       </c>
-      <c r="AY30" s="118">
+      <c r="AY30" s="129">
         <v>52</v>
       </c>
       <c r="AZ30" s="28" t="str">
@@ -34479,7 +34479,7 @@
         <f>MIN(AI26:AI29)</f>
         <v>-3</v>
       </c>
-      <c r="AY31" s="119"/>
+      <c r="AY31" s="130"/>
       <c r="AZ31" s="31" t="str">
         <f>AO21</f>
         <v>2C</v>
@@ -34503,13 +34503,13 @@
       <c r="BN31" s="35"/>
       <c r="BO31" s="36"/>
       <c r="BP31" s="41"/>
-      <c r="BQ31" s="124" t="str">
+      <c r="BQ31" s="131" t="str">
         <f>INDEX(T,7,lang)</f>
         <v>Third-Place Play-Off</v>
       </c>
-      <c r="BR31" s="125"/>
-      <c r="BS31" s="125"/>
-      <c r="BT31" s="126"/>
+      <c r="BR31" s="132"/>
+      <c r="BS31" s="132"/>
+      <c r="BT31" s="133"/>
     </row>
     <row r="32" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18">
@@ -34693,7 +34693,7 @@
       <c r="BH32" s="25"/>
       <c r="BI32" s="36"/>
       <c r="BJ32" s="25"/>
-      <c r="BK32" s="118">
+      <c r="BK32" s="129">
         <v>62</v>
       </c>
       <c r="BL32" s="28" t="str">
@@ -34704,10 +34704,10 @@
       <c r="BN32" s="30"/>
       <c r="BO32" s="40"/>
       <c r="BP32" s="41"/>
-      <c r="BQ32" s="127"/>
-      <c r="BR32" s="128"/>
-      <c r="BS32" s="128"/>
-      <c r="BT32" s="129"/>
+      <c r="BQ32" s="134"/>
+      <c r="BR32" s="135"/>
+      <c r="BS32" s="135"/>
+      <c r="BT32" s="136"/>
     </row>
     <row r="33" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
@@ -34894,7 +34894,7 @@
       <c r="BH33" s="25"/>
       <c r="BI33" s="36"/>
       <c r="BJ33" s="39"/>
-      <c r="BK33" s="119"/>
+      <c r="BK33" s="130"/>
       <c r="BL33" s="31" t="str">
         <f>T72</f>
         <v>W60</v>
@@ -35074,7 +35074,7 @@
         <f>AR34-AS34</f>
         <v>0</v>
       </c>
-      <c r="AY34" s="118">
+      <c r="AY34" s="129">
         <v>55</v>
       </c>
       <c r="AZ34" s="28" t="str">
@@ -35271,7 +35271,7 @@
         <f>AR35-AS35</f>
         <v>0</v>
       </c>
-      <c r="AY35" s="119"/>
+      <c r="AY35" s="130"/>
       <c r="AZ35" s="31" t="str">
         <f>AO33</f>
         <v>2E</v>
@@ -35295,7 +35295,7 @@
       <c r="BN35" s="25"/>
       <c r="BO35" s="25"/>
       <c r="BP35" s="25"/>
-      <c r="BQ35" s="118">
+      <c r="BQ35" s="129">
         <v>63</v>
       </c>
       <c r="BR35" s="28" t="str">
@@ -35457,7 +35457,7 @@
       <c r="BB36" s="25"/>
       <c r="BC36" s="36"/>
       <c r="BD36" s="25"/>
-      <c r="BE36" s="118">
+      <c r="BE36" s="129">
         <v>60</v>
       </c>
       <c r="BF36" s="28" t="str">
@@ -35474,7 +35474,7 @@
       <c r="BN36" s="25"/>
       <c r="BO36" s="25"/>
       <c r="BP36" s="25"/>
-      <c r="BQ36" s="119"/>
+      <c r="BQ36" s="130"/>
       <c r="BR36" s="31" t="str">
         <f>Z77</f>
         <v>L62</v>
@@ -35502,8 +35502,12 @@
         <f>AB50</f>
         <v>Poland</v>
       </c>
-      <c r="F37" s="23"/>
-      <c r="G37" s="24"/>
+      <c r="F37" s="23">
+        <v>0</v>
+      </c>
+      <c r="G37" s="24">
+        <v>3</v>
+      </c>
       <c r="H37" s="67" t="str">
         <f>AB52</f>
         <v>Colombia</v>
@@ -35514,11 +35518,11 @@
       </c>
       <c r="S37" s="65" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Poland_lose</v>
       </c>
       <c r="T37" s="65" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Colombia_win</v>
       </c>
       <c r="U37" s="59">
         <f t="shared" si="4"/>
@@ -35536,9 +35540,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y37" s="58" t="str">
+      <c r="Y37" s="58">
         <f t="shared" si="9"/>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AH37" s="58">
         <f>MIN(AH32:AH35)</f>
@@ -35557,7 +35561,7 @@
       <c r="BB37" s="35"/>
       <c r="BC37" s="36"/>
       <c r="BD37" s="39"/>
-      <c r="BE37" s="119"/>
+      <c r="BE37" s="130"/>
       <c r="BF37" s="31" t="str">
         <f>T65</f>
         <v>W56</v>
@@ -35747,7 +35751,7 @@
         <f>AR38-AS38</f>
         <v>1</v>
       </c>
-      <c r="AY38" s="118">
+      <c r="AY38" s="129">
         <v>56</v>
       </c>
       <c r="AZ38" s="28" t="str">
@@ -35937,7 +35941,7 @@
         <f>AR39-AS39</f>
         <v>0</v>
       </c>
-      <c r="AY39" s="119"/>
+      <c r="AY39" s="130"/>
       <c r="AZ39" s="31" t="str">
         <f>AO45</f>
         <v>2G</v>
@@ -36282,23 +36286,23 @@
         <f>AR41-AS41</f>
         <v>0</v>
       </c>
-      <c r="BJ41" s="120" t="str">
+      <c r="BJ41" s="146" t="str">
         <f>INDEX(T,102,lang)</f>
         <v>World Champion 2018</v>
       </c>
-      <c r="BK41" s="120"/>
-      <c r="BL41" s="120"/>
-      <c r="BM41" s="120"/>
-      <c r="BN41" s="120"/>
-      <c r="BO41" s="122" t="str">
+      <c r="BK41" s="146"/>
+      <c r="BL41" s="146"/>
+      <c r="BM41" s="146"/>
+      <c r="BN41" s="146"/>
+      <c r="BO41" s="148" t="str">
         <f>S85</f>
         <v/>
       </c>
-      <c r="BP41" s="122"/>
-      <c r="BQ41" s="122"/>
-      <c r="BR41" s="122"/>
-      <c r="BS41" s="122"/>
-      <c r="BT41" s="122"/>
+      <c r="BP41" s="148"/>
+      <c r="BQ41" s="148"/>
+      <c r="BR41" s="148"/>
+      <c r="BS41" s="148"/>
+      <c r="BT41" s="148"/>
     </row>
     <row r="42" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18">
@@ -36442,17 +36446,17 @@
         <f>MAX(AT38:AT41)-MIN(AT38:AT41)+1</f>
         <v>3</v>
       </c>
-      <c r="BJ42" s="121"/>
-      <c r="BK42" s="121"/>
-      <c r="BL42" s="121"/>
-      <c r="BM42" s="121"/>
-      <c r="BN42" s="121"/>
-      <c r="BO42" s="123"/>
-      <c r="BP42" s="123"/>
-      <c r="BQ42" s="123"/>
-      <c r="BR42" s="123"/>
-      <c r="BS42" s="123"/>
-      <c r="BT42" s="123"/>
+      <c r="BJ42" s="147"/>
+      <c r="BK42" s="147"/>
+      <c r="BL42" s="147"/>
+      <c r="BM42" s="147"/>
+      <c r="BN42" s="147"/>
+      <c r="BO42" s="149"/>
+      <c r="BP42" s="149"/>
+      <c r="BQ42" s="149"/>
+      <c r="BR42" s="149"/>
+      <c r="BS42" s="149"/>
+      <c r="BT42" s="149"/>
     </row>
     <row r="43" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18">
@@ -37018,12 +37022,12 @@
         <f>AR46-AS46</f>
         <v>0</v>
       </c>
-      <c r="AY46" s="109" t="s">
+      <c r="AY46" s="137" t="s">
         <v>2224</v>
       </c>
-      <c r="AZ46" s="110"/>
-      <c r="BA46" s="110"/>
-      <c r="BB46" s="111"/>
+      <c r="AZ46" s="138"/>
+      <c r="BA46" s="138"/>
+      <c r="BB46" s="139"/>
     </row>
     <row r="47" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18">
@@ -37187,10 +37191,10 @@
         <f>AR47-AS47</f>
         <v>0</v>
       </c>
-      <c r="AY47" s="112"/>
-      <c r="AZ47" s="113"/>
-      <c r="BA47" s="113"/>
-      <c r="BB47" s="114"/>
+      <c r="AY47" s="140"/>
+      <c r="AZ47" s="141"/>
+      <c r="BA47" s="141"/>
+      <c r="BB47" s="142"/>
     </row>
     <row r="48" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18">
@@ -37334,10 +37338,10 @@
         <f>MAX(AT44:AT47)-MIN(AT44:AT47)+1</f>
         <v>1</v>
       </c>
-      <c r="AY48" s="112"/>
-      <c r="AZ48" s="113"/>
-      <c r="BA48" s="113"/>
-      <c r="BB48" s="114"/>
+      <c r="AY48" s="140"/>
+      <c r="AZ48" s="141"/>
+      <c r="BA48" s="141"/>
+      <c r="BB48" s="142"/>
     </row>
     <row r="49" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18">
@@ -37405,10 +37409,10 @@
         <f>MIN(AI44:AI47)</f>
         <v>-8</v>
       </c>
-      <c r="AY49" s="112"/>
-      <c r="AZ49" s="113"/>
-      <c r="BA49" s="113"/>
-      <c r="BB49" s="114"/>
+      <c r="AY49" s="140"/>
+      <c r="AZ49" s="141"/>
+      <c r="BA49" s="141"/>
+      <c r="BB49" s="142"/>
     </row>
     <row r="50" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="18">
@@ -37498,7 +37502,7 @@
       </c>
       <c r="AA50" s="58">
         <f>COUNTIF(AN50:AN53,CONCATENATE("&gt;=",AN50))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB50" s="59" t="str">
         <f>VLOOKUP("Poland",T,lang,FALSE)</f>
@@ -37514,7 +37518,7 @@
       </c>
       <c r="AE50" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB50 &amp; "_lose")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF50" s="58">
         <f>SUMIF($E$7:$E$54,$AB50,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB50,$G$7:$G$54)</f>
@@ -37522,15 +37526,15 @@
       </c>
       <c r="AG50" s="58">
         <f>SUMIF($E$7:$E$54,$AB50,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB50,$F$7:$F$54)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AH50" s="58">
         <f>(AF50-AG50)*100+AK50*10000+AF50</f>
-        <v>-99</v>
+        <v>-399</v>
       </c>
       <c r="AI50" s="58">
         <f>AF50-AG50</f>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="AJ50" s="58">
         <f>(AI50-AI55)/AI54</f>
@@ -37576,10 +37580,10 @@
         <f>AR50-AS50</f>
         <v>0</v>
       </c>
-      <c r="AY50" s="112"/>
-      <c r="AZ50" s="113"/>
-      <c r="BA50" s="113"/>
-      <c r="BB50" s="114"/>
+      <c r="AY50" s="140"/>
+      <c r="AZ50" s="141"/>
+      <c r="BA50" s="141"/>
+      <c r="BB50" s="142"/>
     </row>
     <row r="51" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="18">
@@ -37705,7 +37709,7 @@
       </c>
       <c r="AJ51" s="58">
         <f>(AI51-AI55)/AI54</f>
-        <v>0.66666666666666663</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="AK51" s="58">
         <f>AC51*3+AD51</f>
@@ -37721,7 +37725,7 @@
       </c>
       <c r="AN51" s="59">
         <f>1000*AK51/AK54+100*AJ51+10*AF51/AF54+1*AL51/AL54+AM51</f>
-        <v>877.64775382795699</v>
+        <v>882.40965858986181</v>
       </c>
       <c r="AO51" s="60" t="str">
         <f>IF(SUM(AC50:AE53)=12,J52,INDEX(T,85,lang))</f>
@@ -37747,10 +37751,10 @@
         <f>AR51-AS51</f>
         <v>0</v>
       </c>
-      <c r="AY51" s="112"/>
-      <c r="AZ51" s="113"/>
-      <c r="BA51" s="113"/>
-      <c r="BB51" s="114"/>
+      <c r="AY51" s="140"/>
+      <c r="AZ51" s="141"/>
+      <c r="BA51" s="141"/>
+      <c r="BB51" s="142"/>
     </row>
     <row r="52" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18">
@@ -37840,7 +37844,7 @@
       </c>
       <c r="AA52" s="58">
         <f>COUNTIF(AN50:AN53,CONCATENATE("&gt;=",AN52))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB52" s="59" t="str">
         <f>VLOOKUP("Colombia",T,lang,FALSE)</f>
@@ -37848,7 +37852,7 @@
       </c>
       <c r="AC52" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB52 &amp; "_win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD52" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB52 &amp; "_draw")</f>
@@ -37860,7 +37864,7 @@
       </c>
       <c r="AF52" s="58">
         <f>SUMIF($E$7:$E$54,$AB52,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB52,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AG52" s="58">
         <f>SUMIF($E$7:$E$54,$AB52,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB52,$F$7:$F$54)</f>
@@ -37868,19 +37872,19 @@
       </c>
       <c r="AH52" s="58">
         <f>(AF52-AG52)*100+AK52*10000+AF52</f>
-        <v>-99</v>
+        <v>30204</v>
       </c>
       <c r="AI52" s="58">
         <f>AF52-AG52</f>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AJ52" s="58">
         <f>(AI52-AI55)/AI54</f>
-        <v>0</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="AK52" s="58">
         <f>AC52*3+AD52</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL52" s="58">
         <f>AP52/AP54*1000+AQ52/AQ54*100+AT52/AT54*10+AR52/AR54</f>
@@ -37892,7 +37896,7 @@
       </c>
       <c r="AN52" s="59">
         <f>1000*AK52/AK54+100*AJ52+10*AF52/AF54+1*AL52/AL54+AM52</f>
-        <v>2.5005389999999998</v>
+        <v>695.71482471428567</v>
       </c>
       <c r="AP52" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB52&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB52&amp;"_win")*($U$7:$U$54))</f>
@@ -37914,10 +37918,10 @@
         <f>AR52-AS52</f>
         <v>0</v>
       </c>
-      <c r="AY52" s="115"/>
-      <c r="AZ52" s="116"/>
-      <c r="BA52" s="116"/>
-      <c r="BB52" s="117"/>
+      <c r="AY52" s="143"/>
+      <c r="AZ52" s="144"/>
+      <c r="BA52" s="144"/>
+      <c r="BB52" s="145"/>
     </row>
     <row r="53" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18">
@@ -37947,15 +37951,15 @@
       </c>
       <c r="J53" s="72" t="str">
         <f>VLOOKUP(3,AA50:AK53,2,FALSE)</f>
-        <v>Poland</v>
+        <v>Colombia</v>
       </c>
       <c r="K53" s="27">
         <f>L53+M53+N53</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L53" s="27">
         <f>VLOOKUP(3,AA50:AK53,3,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M53" s="27">
         <f>VLOOKUP(3,AA50:AK53,4,FALSE)</f>
@@ -37967,11 +37971,11 @@
       </c>
       <c r="O53" s="27" t="str">
         <f>VLOOKUP(3,AA50:AK53,6,FALSE) &amp; " - " &amp; VLOOKUP(3,AA50:AK53,7,FALSE)</f>
-        <v>1 - 2</v>
+        <v>4 - 2</v>
       </c>
       <c r="P53" s="73">
         <f>L53*3+M53</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R53" s="58">
         <f>DATE(2018,6,28)+TIME(3,0,0)+gmt_delta</f>
@@ -38043,7 +38047,7 @@
       </c>
       <c r="AJ53" s="58">
         <f>(AI53-AI55)/AI54</f>
-        <v>0.66666666666666663</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="AK53" s="58">
         <f>AC53*3+AD53</f>
@@ -38059,7 +38063,7 @@
       </c>
       <c r="AN53" s="59">
         <f>1000*AK53/AK54+100*AJ53+10*AF53/AF54+1*AL53/AL54+AM53</f>
-        <v>877.64761182795701</v>
+        <v>882.40951658986182</v>
       </c>
       <c r="AP53" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB53&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB53&amp;"_win")*($U$7:$U$54))</f>
@@ -38110,11 +38114,11 @@
       </c>
       <c r="J54" s="74" t="str">
         <f>VLOOKUP(4,AA50:AK53,2,FALSE)</f>
-        <v>Colombia</v>
+        <v>Poland</v>
       </c>
       <c r="K54" s="75">
         <f>L54+M54+N54</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L54" s="75">
         <f>VLOOKUP(4,AA50:AK53,3,FALSE)</f>
@@ -38126,11 +38130,11 @@
       </c>
       <c r="N54" s="75">
         <f>VLOOKUP(4,AA50:AK53,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O54" s="75" t="str">
         <f>VLOOKUP(4,AA50:AK53,6,FALSE) &amp; " - " &amp; VLOOKUP(4,AA50:AK53,7,FALSE)</f>
-        <v>1 - 2</v>
+        <v>1 - 5</v>
       </c>
       <c r="P54" s="76">
         <f>L54*3+M54</f>
@@ -38178,7 +38182,7 @@
       </c>
       <c r="AE54" s="58">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF54" s="58">
         <f t="shared" si="17"/>
@@ -38186,15 +38190,15 @@
       </c>
       <c r="AG54" s="58">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AH54" s="58">
         <f>MAX(AH50:AH53)-AH55+1</f>
-        <v>40204</v>
+        <v>40504</v>
       </c>
       <c r="AI54" s="58">
         <f>MAX(AI50:AI53)-AI55+1</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AK54" s="58">
         <f t="shared" si="17"/>
@@ -38244,11 +38248,11 @@
       <c r="P55" s="49"/>
       <c r="AH55" s="58">
         <f>MIN(AH50:AH53)</f>
-        <v>-99</v>
+        <v>-399</v>
       </c>
       <c r="AI55" s="58">
         <f>MIN(AI50:AI53)</f>
-        <v>-1</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="56" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -38506,27 +38510,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="hexNDhodxxdoIYhe+LOVPFyB2v0aJLQphXCm5lZGwHDaP2ZITl3Lpck5mriyKWgCt8wrzYbwlizwv7dyeeElyw==" saltValue="swcCixFXOL0FnpwQehLBng==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="28">
-    <mergeCell ref="BQ6:BT7"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="A5:H6"/>
-    <mergeCell ref="J5:P6"/>
-    <mergeCell ref="AY10:AY11"/>
-    <mergeCell ref="BE12:BE13"/>
-    <mergeCell ref="AY6:BB7"/>
-    <mergeCell ref="BE6:BH7"/>
-    <mergeCell ref="BK6:BN7"/>
-    <mergeCell ref="AY22:AY23"/>
-    <mergeCell ref="BQ23:BQ24"/>
-    <mergeCell ref="AY18:AY19"/>
-    <mergeCell ref="BE20:BE21"/>
-    <mergeCell ref="AY14:AY15"/>
-    <mergeCell ref="BK16:BK17"/>
-    <mergeCell ref="AY30:AY31"/>
-    <mergeCell ref="BQ31:BT32"/>
-    <mergeCell ref="BK32:BK33"/>
-    <mergeCell ref="AY26:AY27"/>
-    <mergeCell ref="BE28:BE29"/>
     <mergeCell ref="AY46:BB52"/>
     <mergeCell ref="AY38:AY39"/>
     <mergeCell ref="BJ41:BN42"/>
@@ -38534,6 +38517,27 @@
     <mergeCell ref="BQ35:BQ36"/>
     <mergeCell ref="BE36:BE37"/>
     <mergeCell ref="BO41:BT42"/>
+    <mergeCell ref="AY30:AY31"/>
+    <mergeCell ref="BQ31:BT32"/>
+    <mergeCell ref="BK32:BK33"/>
+    <mergeCell ref="AY26:AY27"/>
+    <mergeCell ref="BE28:BE29"/>
+    <mergeCell ref="AY22:AY23"/>
+    <mergeCell ref="BQ23:BQ24"/>
+    <mergeCell ref="AY18:AY19"/>
+    <mergeCell ref="BE20:BE21"/>
+    <mergeCell ref="AY14:AY15"/>
+    <mergeCell ref="BK16:BK17"/>
+    <mergeCell ref="AY10:AY11"/>
+    <mergeCell ref="BE12:BE13"/>
+    <mergeCell ref="AY6:BB7"/>
+    <mergeCell ref="BE6:BH7"/>
+    <mergeCell ref="BK6:BN7"/>
+    <mergeCell ref="BQ6:BT7"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="A5:H6"/>
+    <mergeCell ref="J5:P6"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="F7:F55">

</xml_diff>

<commit_message>
Add Jennifer and update for final score
</commit_message>
<xml_diff>
--- a/input/world_cup_2018_final.xlsx
+++ b/input/world_cup_2018_final.xlsx
@@ -9316,6 +9316,90 @@
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -9394,90 +9478,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -29896,8 +29896,8 @@
   </sheetPr>
   <dimension ref="A1:BT97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -29952,25 +29952,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:72" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="115" t="str">
+      <c r="A1" s="136" t="str">
         <f>INDEX(T,2,lang)</f>
         <v>2018 World Cup Final Tournament Schedule</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="136"/>
+      <c r="M1" s="136"/>
+      <c r="N1" s="136"/>
+      <c r="O1" s="136"/>
+      <c r="P1" s="136"/>
       <c r="S1" s="58"/>
       <c r="T1" s="58"/>
       <c r="U1" s="58"/>
@@ -30033,11 +30033,11 @@
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
-      <c r="O3" s="116" t="str">
+      <c r="O3" s="137" t="str">
         <f>"Language: " &amp; Settings!C4</f>
         <v>Language: English</v>
       </c>
-      <c r="P3" s="116"/>
+      <c r="P3" s="137"/>
       <c r="S3" s="58"/>
       <c r="T3" s="58"/>
       <c r="U3" s="58"/>
@@ -30063,43 +30063,43 @@
     </row>
     <row r="4" spans="1:72" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="117" t="str">
+      <c r="A5" s="138" t="str">
         <f>INDEX(T,3,lang)</f>
         <v>Group Stage</v>
       </c>
-      <c r="B5" s="118"/>
-      <c r="C5" s="118"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="119"/>
-      <c r="J5" s="123" t="s">
+      <c r="B5" s="139"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="139"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="140"/>
+      <c r="J5" s="144" t="s">
         <v>2174</v>
       </c>
-      <c r="K5" s="124"/>
-      <c r="L5" s="124"/>
-      <c r="M5" s="124"/>
-      <c r="N5" s="124"/>
-      <c r="O5" s="124"/>
-      <c r="P5" s="125"/>
+      <c r="K5" s="145"/>
+      <c r="L5" s="145"/>
+      <c r="M5" s="145"/>
+      <c r="N5" s="145"/>
+      <c r="O5" s="145"/>
+      <c r="P5" s="146"/>
     </row>
     <row r="6" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="120"/>
-      <c r="B6" s="121"/>
-      <c r="C6" s="121"/>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="121"/>
-      <c r="H6" s="122"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="127"/>
-      <c r="M6" s="127"/>
-      <c r="N6" s="127"/>
-      <c r="O6" s="127"/>
-      <c r="P6" s="128"/>
+      <c r="A6" s="141"/>
+      <c r="B6" s="142"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="142"/>
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="143"/>
+      <c r="J6" s="147"/>
+      <c r="K6" s="148"/>
+      <c r="L6" s="148"/>
+      <c r="M6" s="148"/>
+      <c r="N6" s="148"/>
+      <c r="O6" s="148"/>
+      <c r="P6" s="149"/>
       <c r="R6" s="58" t="s">
         <v>2175</v>
       </c>
@@ -30163,34 +30163,34 @@
       <c r="AT6" s="62" t="s">
         <v>2182</v>
       </c>
-      <c r="AY6" s="109" t="str">
+      <c r="AY6" s="130" t="str">
         <f>INDEX(T,4,lang)</f>
         <v>Round of 16</v>
       </c>
-      <c r="AZ6" s="110"/>
-      <c r="BA6" s="110"/>
-      <c r="BB6" s="111"/>
-      <c r="BE6" s="109" t="str">
+      <c r="AZ6" s="131"/>
+      <c r="BA6" s="131"/>
+      <c r="BB6" s="132"/>
+      <c r="BE6" s="130" t="str">
         <f>INDEX(T,5,lang)</f>
         <v>Quarterfinals</v>
       </c>
-      <c r="BF6" s="110"/>
-      <c r="BG6" s="110"/>
-      <c r="BH6" s="111"/>
-      <c r="BK6" s="109" t="str">
+      <c r="BF6" s="131"/>
+      <c r="BG6" s="131"/>
+      <c r="BH6" s="132"/>
+      <c r="BK6" s="130" t="str">
         <f>INDEX(T,6,lang)</f>
         <v>Semi-Finals</v>
       </c>
-      <c r="BL6" s="110"/>
-      <c r="BM6" s="110"/>
-      <c r="BN6" s="111"/>
-      <c r="BQ6" s="109" t="str">
+      <c r="BL6" s="131"/>
+      <c r="BM6" s="131"/>
+      <c r="BN6" s="132"/>
+      <c r="BQ6" s="130" t="str">
         <f>INDEX(T,8,lang)</f>
         <v>Final</v>
       </c>
-      <c r="BR6" s="110"/>
-      <c r="BS6" s="110"/>
-      <c r="BT6" s="111"/>
+      <c r="BR6" s="131"/>
+      <c r="BS6" s="131"/>
+      <c r="BT6" s="132"/>
     </row>
     <row r="7" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
@@ -30254,22 +30254,22 @@
         <f>IF(OR(F7="",G7=""),"",IF(F7&gt;G7,1,IF(F7&lt;G7,-1,0)))</f>
         <v>1</v>
       </c>
-      <c r="AY7" s="112"/>
-      <c r="AZ7" s="113"/>
-      <c r="BA7" s="113"/>
-      <c r="BB7" s="114"/>
-      <c r="BE7" s="112"/>
-      <c r="BF7" s="113"/>
-      <c r="BG7" s="113"/>
-      <c r="BH7" s="114"/>
-      <c r="BK7" s="112"/>
-      <c r="BL7" s="113"/>
-      <c r="BM7" s="113"/>
-      <c r="BN7" s="114"/>
-      <c r="BQ7" s="112"/>
-      <c r="BR7" s="113"/>
-      <c r="BS7" s="113"/>
-      <c r="BT7" s="114"/>
+      <c r="AY7" s="133"/>
+      <c r="AZ7" s="134"/>
+      <c r="BA7" s="134"/>
+      <c r="BB7" s="135"/>
+      <c r="BE7" s="133"/>
+      <c r="BF7" s="134"/>
+      <c r="BG7" s="134"/>
+      <c r="BH7" s="135"/>
+      <c r="BK7" s="133"/>
+      <c r="BL7" s="134"/>
+      <c r="BM7" s="134"/>
+      <c r="BN7" s="135"/>
+      <c r="BQ7" s="133"/>
+      <c r="BR7" s="134"/>
+      <c r="BS7" s="134"/>
+      <c r="BT7" s="135"/>
     </row>
     <row r="8" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
@@ -30363,7 +30363,7 @@
       </c>
       <c r="AA8" s="58">
         <f>COUNTIF(AN8:AN11,CONCATENATE("&gt;=",AN8))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB8" s="59" t="str">
         <f>VLOOKUP("Russia",T,lang,FALSE)</f>
@@ -30379,7 +30379,7 @@
       </c>
       <c r="AE8" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB8 &amp; "_lose")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF8" s="58">
         <f>SUMIF($E$7:$E$54,$AB8,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB8,$G$7:$G$54)</f>
@@ -30387,19 +30387,19 @@
       </c>
       <c r="AG8" s="58">
         <f>SUMIF($E$7:$E$54,$AB8,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB8,$F$7:$F$54)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AH8" s="58">
         <f>(AF8-AG8)+1</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AI8" s="58">
         <f>AF8-AG8</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AJ8" s="58">
         <f>(AI8-AI13)/AI12</f>
-        <v>0.9285714285714286</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="AK8" s="58">
         <f>AC8*3+AD8</f>
@@ -30415,11 +30415,11 @@
       </c>
       <c r="AN8" s="59">
         <f>1000*AK8/AK12+100*AJ8+10*AF8/AF12+1*AL8/AL12+AM8</f>
-        <v>958.88915588888892</v>
+        <v>693.24702024675332</v>
       </c>
       <c r="AO8" s="60" t="str">
         <f>IF(SUM(AC8:AE11)=12,J9,INDEX(T,70,lang))</f>
-        <v>1A</v>
+        <v>Uruguay</v>
       </c>
       <c r="AP8" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB8&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB8&amp;"_win")*($U$7:$U$54))</f>
@@ -30485,15 +30485,15 @@
       </c>
       <c r="J9" s="69" t="str">
         <f>VLOOKUP(1,AA8:AK11,2,FALSE)</f>
-        <v>Russia</v>
+        <v>Uruguay</v>
       </c>
       <c r="K9" s="70">
         <f>L9+M9+N9</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L9" s="70">
         <f>VLOOKUP(1,AA8:AK11,3,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M9" s="70">
         <f>VLOOKUP(1,AA8:AK11,4,FALSE)</f>
@@ -30505,11 +30505,11 @@
       </c>
       <c r="O9" s="70" t="str">
         <f>VLOOKUP(1,AA8:AK11,6,FALSE) &amp; " - " &amp; VLOOKUP(1,AA8:AK11,7,FALSE)</f>
-        <v>8 - 1</v>
+        <v>5 - 0</v>
       </c>
       <c r="P9" s="71">
         <f>L9*3+M9</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="R9" s="58">
         <f>DATE(2018,6,15)+TIME(7,0,0)+gmt_delta</f>
@@ -30545,7 +30545,7 @@
       </c>
       <c r="AA9" s="58">
         <f>COUNTIF(AN8:AN11,CONCATENATE("&gt;=",AN9))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB9" s="59" t="str">
         <f>VLOOKUP("Saudi Arabia",T,lang,FALSE)</f>
@@ -30553,7 +30553,7 @@
       </c>
       <c r="AC9" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB9 &amp; "_win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD9" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB9 &amp; "_draw")</f>
@@ -30565,19 +30565,19 @@
       </c>
       <c r="AF9" s="58">
         <f>SUMIF($E$7:$E$54,$AB9,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB9,$G$7:$G$54)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG9" s="58">
         <f>SUMIF($E$7:$E$54,$AB9,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB9,$F$7:$F$54)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AH9" s="58">
         <f>(AF9-AG9)+1</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="AI9" s="58">
         <f>AF9-AG9</f>
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="AJ9" s="58">
         <f>(AI9-AI13)/AI12</f>
@@ -30585,7 +30585,7 @@
       </c>
       <c r="AK9" s="58">
         <f>AC9*3+AD9</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL9" s="58">
         <f>AP9/AP12*1000+AQ9/AQ12*100+AT9/AT12*10+AR9/AR12</f>
@@ -30597,11 +30597,11 @@
       </c>
       <c r="AN9" s="59">
         <f>1000*AK9/AK12+100*AJ9+10*AF9/AF12+1*AL9/AL12+AM9</f>
-        <v>2.7149999999999999E-4</v>
+        <v>302.85741435714283</v>
       </c>
       <c r="AO9" s="60" t="str">
         <f>IF(SUM(AC8:AE11)=12,J10,INDEX(T,71,lang))</f>
-        <v>2A</v>
+        <v>Russia</v>
       </c>
       <c r="AP9" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB9&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB9&amp;"_win")*($U$7:$U$54))</f>
@@ -30681,11 +30681,11 @@
       </c>
       <c r="J10" s="72" t="str">
         <f>VLOOKUP(2,AA8:AK11,2,FALSE)</f>
-        <v>Uruguay</v>
+        <v>Russia</v>
       </c>
       <c r="K10" s="27">
         <f>L10+M10+N10</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L10" s="27">
         <f>VLOOKUP(2,AA8:AK11,3,FALSE)</f>
@@ -30697,11 +30697,11 @@
       </c>
       <c r="N10" s="27">
         <f>VLOOKUP(2,AA8:AK11,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10" s="27" t="str">
         <f>VLOOKUP(2,AA8:AK11,6,FALSE) &amp; " - " &amp; VLOOKUP(2,AA8:AK11,7,FALSE)</f>
-        <v>2 - 0</v>
+        <v>8 - 4</v>
       </c>
       <c r="P10" s="73">
         <f>L10*3+M10</f>
@@ -30741,7 +30741,7 @@
       </c>
       <c r="AA10" s="58">
         <f>COUNTIF(AN8:AN11,CONCATENATE("&gt;=",AN10))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB10" s="59" t="str">
         <f>VLOOKUP("Egypt",T,lang,FALSE)</f>
@@ -30757,27 +30757,27 @@
       </c>
       <c r="AE10" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB10 &amp; "_lose")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF10" s="58">
         <f>SUMIF($E$7:$E$54,$AB10,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB10,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG10" s="58">
         <f>SUMIF($E$7:$E$54,$AB10,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB10,$F$7:$F$54)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AH10" s="58">
         <f>(AF10-AG10)+1</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AI10" s="58">
         <f>AF10-AG10</f>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="AJ10" s="58">
         <f>(AI10-AI13)/AI12</f>
-        <v>0.21428571428571427</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AK10" s="58">
         <f>AC10*3+AD10</f>
@@ -30793,7 +30793,7 @@
       </c>
       <c r="AN10" s="59">
         <f>1000*AK10/AK12+100*AJ10+10*AF10/AF12+1*AL10/AL12+AM10</f>
-        <v>22.540085039682538</v>
+        <v>11.948454448051949</v>
       </c>
       <c r="AP10" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB10&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB10&amp;"_win")*($U$7:$U$54))</f>
@@ -30815,12 +30815,12 @@
         <f>AR10-AS10</f>
         <v>0</v>
       </c>
-      <c r="AY10" s="129">
+      <c r="AY10" s="118">
         <v>49</v>
       </c>
       <c r="AZ10" s="28" t="str">
         <f>AO8</f>
-        <v>1A</v>
+        <v>Uruguay</v>
       </c>
       <c r="BA10" s="29"/>
       <c r="BB10" s="30"/>
@@ -30875,15 +30875,15 @@
       </c>
       <c r="J11" s="72" t="str">
         <f>VLOOKUP(3,AA8:AK11,2,FALSE)</f>
-        <v>Egypt</v>
+        <v>Saudi Arabia</v>
       </c>
       <c r="K11" s="27">
         <f>L11+M11+N11</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L11" s="27">
         <f>VLOOKUP(3,AA8:AK11,3,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="27">
         <f>VLOOKUP(3,AA8:AK11,4,FALSE)</f>
@@ -30895,11 +30895,11 @@
       </c>
       <c r="O11" s="27" t="str">
         <f>VLOOKUP(3,AA8:AK11,6,FALSE) &amp; " - " &amp; VLOOKUP(3,AA8:AK11,7,FALSE)</f>
-        <v>1 - 4</v>
+        <v>2 - 7</v>
       </c>
       <c r="P11" s="73">
         <f>L11*3+M11</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R11" s="58">
         <f>DATE(2018,6,15)+TIME(23,0,0)+gmt_delta</f>
@@ -30935,7 +30935,7 @@
       </c>
       <c r="AA11" s="58">
         <f>COUNTIF(AN8:AN11,CONCATENATE("&gt;=",AN11))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB11" s="59" t="str">
         <f>VLOOKUP("Uruguay",T,lang,FALSE)</f>
@@ -30943,7 +30943,7 @@
       </c>
       <c r="AC11" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB11 &amp; "_win")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD11" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB11 &amp; "_draw")</f>
@@ -30955,7 +30955,7 @@
       </c>
       <c r="AF11" s="58">
         <f>SUMIF($E$7:$E$54,$AB11,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB11,$G$7:$G$54)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AG11" s="58">
         <f>SUMIF($E$7:$E$54,$AB11,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB11,$F$7:$F$54)</f>
@@ -30963,19 +30963,19 @@
       </c>
       <c r="AH11" s="58">
         <f>(AF11-AG11)+1</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AI11" s="58">
         <f>AF11-AG11</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AJ11" s="58">
         <f>(AI11-AI13)/AI12</f>
-        <v>0.5714285714285714</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="AK11" s="58">
         <f>AC11*3+AD11</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AL11" s="58">
         <f>AP11/AP12*1000+AQ11/AQ12*100+AT11/AT12*10+AR11/AR12</f>
@@ -30987,7 +30987,7 @@
       </c>
       <c r="AN11" s="59">
         <f>1000*AK11/AK12+100*AJ11+10*AF11/AF12+1*AL11/AL12+AM11</f>
-        <v>916.50839850793636</v>
+        <v>998.05241005194796</v>
       </c>
       <c r="AP11" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB11&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB11&amp;"_win")*($U$7:$U$54))</f>
@@ -31009,7 +31009,7 @@
         <f>AR11-AS11</f>
         <v>0</v>
       </c>
-      <c r="AY11" s="130"/>
+      <c r="AY11" s="119"/>
       <c r="AZ11" s="31" t="str">
         <f>AO15</f>
         <v>2B</v>
@@ -31070,11 +31070,11 @@
       </c>
       <c r="J12" s="74" t="str">
         <f>VLOOKUP(4,AA8:AK11,2,FALSE)</f>
-        <v>Saudi Arabia</v>
+        <v>Egypt</v>
       </c>
       <c r="K12" s="75">
         <f>L12+M12+N12</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L12" s="75">
         <f>VLOOKUP(4,AA8:AK11,3,FALSE)</f>
@@ -31086,11 +31086,11 @@
       </c>
       <c r="N12" s="75">
         <f>VLOOKUP(4,AA8:AK11,5,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O12" s="75" t="str">
         <f>VLOOKUP(4,AA8:AK11,6,FALSE) &amp; " - " &amp; VLOOKUP(4,AA8:AK11,7,FALSE)</f>
-        <v>0 - 6</v>
+        <v>2 - 6</v>
       </c>
       <c r="P12" s="76">
         <f>L12*3+M12</f>
@@ -31130,7 +31130,7 @@
       </c>
       <c r="AC12" s="58">
         <f t="shared" ref="AC12:AL12" si="10">MAX(AC8:AC11)-MIN(AC8:AC11)+1</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AD12" s="58">
         <f t="shared" si="10"/>
@@ -31138,27 +31138,27 @@
       </c>
       <c r="AE12" s="58">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AF12" s="58">
         <f t="shared" si="10"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AG12" s="58">
         <f t="shared" si="10"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AH12" s="58">
         <f>MAX(AH8:AH11)-AH13+1</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="AI12" s="58">
         <f>MAX(AI8:AI11)-AI13+1</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="AK12" s="58">
         <f t="shared" si="10"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AL12" s="58">
         <f t="shared" si="10"/>
@@ -31190,7 +31190,7 @@
       <c r="BB12" s="25"/>
       <c r="BC12" s="36"/>
       <c r="BD12" s="25"/>
-      <c r="BE12" s="129">
+      <c r="BE12" s="118">
         <v>57</v>
       </c>
       <c r="BF12" s="28" t="str">
@@ -31283,11 +31283,11 @@
       </c>
       <c r="AH13" s="58">
         <f>MIN(AH8:AH11)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="AI13" s="58">
         <f>MIN(AI8:AI11)</f>
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="AY13" s="25" t="str">
         <f>INDEX(T,24+MONTH(R59),lang) &amp; " " &amp; DAY(R59) &amp; ", " &amp; YEAR(R59) &amp; "   " &amp; (IF(HOUR(R59)&lt;10,0,"")&amp;HOUR(R59)) &amp; ":" &amp;  (IF(MINUTE(R59)&lt;10,0,"")&amp;MINUTE(R59))</f>
@@ -31298,7 +31298,7 @@
       <c r="BB13" s="35"/>
       <c r="BC13" s="36"/>
       <c r="BD13" s="39"/>
-      <c r="BE13" s="130"/>
+      <c r="BE13" s="119"/>
       <c r="BF13" s="31" t="str">
         <f>T59</f>
         <v>W50</v>
@@ -31488,7 +31488,7 @@
         <f>AR14-AS14</f>
         <v>0</v>
       </c>
-      <c r="AY14" s="129">
+      <c r="AY14" s="118">
         <v>50</v>
       </c>
       <c r="AZ14" s="28" t="str">
@@ -31686,7 +31686,7 @@
         <f>AR15-AS15</f>
         <v>0</v>
       </c>
-      <c r="AY15" s="130"/>
+      <c r="AY15" s="119"/>
       <c r="AZ15" s="31" t="str">
         <f>AO27</f>
         <v>2D</v>
@@ -31893,7 +31893,7 @@
       <c r="BH16" s="25"/>
       <c r="BI16" s="36"/>
       <c r="BJ16" s="25"/>
-      <c r="BK16" s="129">
+      <c r="BK16" s="118">
         <v>61</v>
       </c>
       <c r="BL16" s="28" t="str">
@@ -32090,7 +32090,7 @@
       <c r="BH17" s="25"/>
       <c r="BI17" s="36"/>
       <c r="BJ17" s="39"/>
-      <c r="BK17" s="130"/>
+      <c r="BK17" s="119"/>
       <c r="BL17" s="31" t="str">
         <f>T70</f>
         <v>W58</v>
@@ -32250,7 +32250,7 @@
         <f>MAX(AT14:AT17)-MIN(AT14:AT17)+1</f>
         <v>1</v>
       </c>
-      <c r="AY18" s="129">
+      <c r="AY18" s="118">
         <v>53</v>
       </c>
       <c r="AZ18" s="28" t="str">
@@ -32355,7 +32355,7 @@
         <f>MIN(AI14:AI17)</f>
         <v>-2</v>
       </c>
-      <c r="AY19" s="130"/>
+      <c r="AY19" s="119"/>
       <c r="AZ19" s="31" t="str">
         <f>AO39</f>
         <v>2F</v>
@@ -32560,7 +32560,7 @@
       <c r="BB20" s="25"/>
       <c r="BC20" s="36"/>
       <c r="BD20" s="25"/>
-      <c r="BE20" s="129">
+      <c r="BE20" s="118">
         <v>58</v>
       </c>
       <c r="BF20" s="28" t="str">
@@ -32761,7 +32761,7 @@
       <c r="BB21" s="35"/>
       <c r="BC21" s="36"/>
       <c r="BD21" s="39"/>
-      <c r="BE21" s="130"/>
+      <c r="BE21" s="119"/>
       <c r="BF21" s="31" t="str">
         <f>T63</f>
         <v>W54</v>
@@ -32947,7 +32947,7 @@
         <f>AR22-AS22</f>
         <v>0</v>
       </c>
-      <c r="AY22" s="129">
+      <c r="AY22" s="118">
         <v>54</v>
       </c>
       <c r="AZ22" s="28" t="str">
@@ -33144,7 +33144,7 @@
         <f>AR23-AS23</f>
         <v>0</v>
       </c>
-      <c r="AY23" s="130"/>
+      <c r="AY23" s="119"/>
       <c r="AZ23" s="31" t="str">
         <f>AO51</f>
         <v>2H</v>
@@ -33165,7 +33165,7 @@
       <c r="BN23" s="25"/>
       <c r="BO23" s="36"/>
       <c r="BP23" s="25"/>
-      <c r="BQ23" s="129">
+      <c r="BQ23" s="118">
         <v>64</v>
       </c>
       <c r="BR23" s="28" t="str">
@@ -33338,7 +33338,7 @@
       <c r="BN24" s="25"/>
       <c r="BO24" s="36"/>
       <c r="BP24" s="39"/>
-      <c r="BQ24" s="130"/>
+      <c r="BQ24" s="119"/>
       <c r="BR24" s="31" t="str">
         <f>T77</f>
         <v>W62</v>
@@ -33619,7 +33619,7 @@
         <f>AR26-AS26</f>
         <v>0</v>
       </c>
-      <c r="AY26" s="129">
+      <c r="AY26" s="118">
         <v>51</v>
       </c>
       <c r="AZ26" s="28" t="str">
@@ -33817,10 +33817,10 @@
         <f>AR27-AS27</f>
         <v>0</v>
       </c>
-      <c r="AY27" s="130"/>
+      <c r="AY27" s="119"/>
       <c r="AZ27" s="31" t="str">
         <f>AO9</f>
-        <v>2A</v>
+        <v>Russia</v>
       </c>
       <c r="BA27" s="32"/>
       <c r="BB27" s="33"/>
@@ -34018,7 +34018,7 @@
       <c r="BB28" s="25"/>
       <c r="BC28" s="36"/>
       <c r="BD28" s="25"/>
-      <c r="BE28" s="129">
+      <c r="BE28" s="118">
         <v>59</v>
       </c>
       <c r="BF28" s="28" t="str">
@@ -34215,7 +34215,7 @@
       <c r="BB29" s="35"/>
       <c r="BC29" s="36"/>
       <c r="BD29" s="39"/>
-      <c r="BE29" s="130"/>
+      <c r="BE29" s="119"/>
       <c r="BF29" s="31" t="str">
         <f>T61</f>
         <v>W52</v>
@@ -34381,7 +34381,7 @@
         <f>MAX(AT26:AT29)-MIN(AT26:AT29)+1</f>
         <v>1</v>
       </c>
-      <c r="AY30" s="129">
+      <c r="AY30" s="118">
         <v>52</v>
       </c>
       <c r="AZ30" s="28" t="str">
@@ -34479,7 +34479,7 @@
         <f>MIN(AI26:AI29)</f>
         <v>-3</v>
       </c>
-      <c r="AY31" s="130"/>
+      <c r="AY31" s="119"/>
       <c r="AZ31" s="31" t="str">
         <f>AO21</f>
         <v>2C</v>
@@ -34503,13 +34503,13 @@
       <c r="BN31" s="35"/>
       <c r="BO31" s="36"/>
       <c r="BP31" s="41"/>
-      <c r="BQ31" s="131" t="str">
+      <c r="BQ31" s="124" t="str">
         <f>INDEX(T,7,lang)</f>
         <v>Third-Place Play-Off</v>
       </c>
-      <c r="BR31" s="132"/>
-      <c r="BS31" s="132"/>
-      <c r="BT31" s="133"/>
+      <c r="BR31" s="125"/>
+      <c r="BS31" s="125"/>
+      <c r="BT31" s="126"/>
     </row>
     <row r="32" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18">
@@ -34693,7 +34693,7 @@
       <c r="BH32" s="25"/>
       <c r="BI32" s="36"/>
       <c r="BJ32" s="25"/>
-      <c r="BK32" s="129">
+      <c r="BK32" s="118">
         <v>62</v>
       </c>
       <c r="BL32" s="28" t="str">
@@ -34704,10 +34704,10 @@
       <c r="BN32" s="30"/>
       <c r="BO32" s="40"/>
       <c r="BP32" s="41"/>
-      <c r="BQ32" s="134"/>
-      <c r="BR32" s="135"/>
-      <c r="BS32" s="135"/>
-      <c r="BT32" s="136"/>
+      <c r="BQ32" s="127"/>
+      <c r="BR32" s="128"/>
+      <c r="BS32" s="128"/>
+      <c r="BT32" s="129"/>
     </row>
     <row r="33" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
@@ -34894,7 +34894,7 @@
       <c r="BH33" s="25"/>
       <c r="BI33" s="36"/>
       <c r="BJ33" s="39"/>
-      <c r="BK33" s="130"/>
+      <c r="BK33" s="119"/>
       <c r="BL33" s="31" t="str">
         <f>T72</f>
         <v>W60</v>
@@ -35074,7 +35074,7 @@
         <f>AR34-AS34</f>
         <v>0</v>
       </c>
-      <c r="AY34" s="129">
+      <c r="AY34" s="118">
         <v>55</v>
       </c>
       <c r="AZ34" s="28" t="str">
@@ -35271,7 +35271,7 @@
         <f>AR35-AS35</f>
         <v>0</v>
       </c>
-      <c r="AY35" s="130"/>
+      <c r="AY35" s="119"/>
       <c r="AZ35" s="31" t="str">
         <f>AO33</f>
         <v>2E</v>
@@ -35295,7 +35295,7 @@
       <c r="BN35" s="25"/>
       <c r="BO35" s="25"/>
       <c r="BP35" s="25"/>
-      <c r="BQ35" s="129">
+      <c r="BQ35" s="118">
         <v>63</v>
       </c>
       <c r="BR35" s="28" t="str">
@@ -35457,7 +35457,7 @@
       <c r="BB36" s="25"/>
       <c r="BC36" s="36"/>
       <c r="BD36" s="25"/>
-      <c r="BE36" s="129">
+      <c r="BE36" s="118">
         <v>60</v>
       </c>
       <c r="BF36" s="28" t="str">
@@ -35474,7 +35474,7 @@
       <c r="BN36" s="25"/>
       <c r="BO36" s="25"/>
       <c r="BP36" s="25"/>
-      <c r="BQ36" s="130"/>
+      <c r="BQ36" s="119"/>
       <c r="BR36" s="31" t="str">
         <f>Z77</f>
         <v>L62</v>
@@ -35561,7 +35561,7 @@
       <c r="BB37" s="35"/>
       <c r="BC37" s="36"/>
       <c r="BD37" s="39"/>
-      <c r="BE37" s="130"/>
+      <c r="BE37" s="119"/>
       <c r="BF37" s="31" t="str">
         <f>T65</f>
         <v>W56</v>
@@ -35751,7 +35751,7 @@
         <f>AR38-AS38</f>
         <v>1</v>
       </c>
-      <c r="AY38" s="129">
+      <c r="AY38" s="118">
         <v>56</v>
       </c>
       <c r="AZ38" s="28" t="str">
@@ -35795,8 +35795,12 @@
         <f>AB11</f>
         <v>Uruguay</v>
       </c>
-      <c r="F39" s="23"/>
-      <c r="G39" s="24"/>
+      <c r="F39" s="23">
+        <v>3</v>
+      </c>
+      <c r="G39" s="24">
+        <v>0</v>
+      </c>
       <c r="H39" s="67" t="str">
         <f>AB8</f>
         <v>Russia</v>
@@ -35835,11 +35839,11 @@
       </c>
       <c r="S39" s="65" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Uruguay_win</v>
       </c>
       <c r="T39" s="65" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Russia_lose</v>
       </c>
       <c r="U39" s="59">
         <f t="shared" si="4"/>
@@ -35857,9 +35861,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y39" s="58" t="str">
+      <c r="Y39" s="58">
         <f t="shared" si="9"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AA39" s="58">
         <f>COUNTIF(AN38:AN41,CONCATENATE("&gt;=",AN39))</f>
@@ -35941,7 +35945,7 @@
         <f>AR39-AS39</f>
         <v>0</v>
       </c>
-      <c r="AY39" s="130"/>
+      <c r="AY39" s="119"/>
       <c r="AZ39" s="31" t="str">
         <f>AO45</f>
         <v>2G</v>
@@ -35981,8 +35985,12 @@
         <f>AB9</f>
         <v>Saudi Arabia</v>
       </c>
-      <c r="F40" s="23"/>
-      <c r="G40" s="24"/>
+      <c r="F40" s="23">
+        <v>2</v>
+      </c>
+      <c r="G40" s="24">
+        <v>1</v>
+      </c>
       <c r="H40" s="67" t="str">
         <f>AB10</f>
         <v>Egypt</v>
@@ -36021,11 +36029,11 @@
       </c>
       <c r="S40" s="65" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Saudi Arabia_win</v>
       </c>
       <c r="T40" s="65" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Egypt_lose</v>
       </c>
       <c r="U40" s="59">
         <f t="shared" si="4"/>
@@ -36043,9 +36051,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y40" s="58" t="str">
+      <c r="Y40" s="58">
         <f t="shared" si="9"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AA40" s="58">
         <f>COUNTIF(AN38:AN41,CONCATENATE("&gt;=",AN40))</f>
@@ -36286,23 +36294,23 @@
         <f>AR41-AS41</f>
         <v>0</v>
       </c>
-      <c r="BJ41" s="146" t="str">
+      <c r="BJ41" s="120" t="str">
         <f>INDEX(T,102,lang)</f>
         <v>World Champion 2018</v>
       </c>
-      <c r="BK41" s="146"/>
-      <c r="BL41" s="146"/>
-      <c r="BM41" s="146"/>
-      <c r="BN41" s="146"/>
-      <c r="BO41" s="148" t="str">
+      <c r="BK41" s="120"/>
+      <c r="BL41" s="120"/>
+      <c r="BM41" s="120"/>
+      <c r="BN41" s="120"/>
+      <c r="BO41" s="122" t="str">
         <f>S85</f>
         <v/>
       </c>
-      <c r="BP41" s="148"/>
-      <c r="BQ41" s="148"/>
-      <c r="BR41" s="148"/>
-      <c r="BS41" s="148"/>
-      <c r="BT41" s="148"/>
+      <c r="BP41" s="122"/>
+      <c r="BQ41" s="122"/>
+      <c r="BR41" s="122"/>
+      <c r="BS41" s="122"/>
+      <c r="BT41" s="122"/>
     </row>
     <row r="42" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18">
@@ -36446,17 +36454,17 @@
         <f>MAX(AT38:AT41)-MIN(AT38:AT41)+1</f>
         <v>3</v>
       </c>
-      <c r="BJ42" s="147"/>
-      <c r="BK42" s="147"/>
-      <c r="BL42" s="147"/>
-      <c r="BM42" s="147"/>
-      <c r="BN42" s="147"/>
-      <c r="BO42" s="149"/>
-      <c r="BP42" s="149"/>
-      <c r="BQ42" s="149"/>
-      <c r="BR42" s="149"/>
-      <c r="BS42" s="149"/>
-      <c r="BT42" s="149"/>
+      <c r="BJ42" s="121"/>
+      <c r="BK42" s="121"/>
+      <c r="BL42" s="121"/>
+      <c r="BM42" s="121"/>
+      <c r="BN42" s="121"/>
+      <c r="BO42" s="123"/>
+      <c r="BP42" s="123"/>
+      <c r="BQ42" s="123"/>
+      <c r="BR42" s="123"/>
+      <c r="BS42" s="123"/>
+      <c r="BT42" s="123"/>
     </row>
     <row r="43" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18">
@@ -37022,12 +37030,12 @@
         <f>AR46-AS46</f>
         <v>0</v>
       </c>
-      <c r="AY46" s="137" t="s">
+      <c r="AY46" s="109" t="s">
         <v>2224</v>
       </c>
-      <c r="AZ46" s="138"/>
-      <c r="BA46" s="138"/>
-      <c r="BB46" s="139"/>
+      <c r="AZ46" s="110"/>
+      <c r="BA46" s="110"/>
+      <c r="BB46" s="111"/>
     </row>
     <row r="47" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18">
@@ -37191,10 +37199,10 @@
         <f>AR47-AS47</f>
         <v>0</v>
       </c>
-      <c r="AY47" s="140"/>
-      <c r="AZ47" s="141"/>
-      <c r="BA47" s="141"/>
-      <c r="BB47" s="142"/>
+      <c r="AY47" s="112"/>
+      <c r="AZ47" s="113"/>
+      <c r="BA47" s="113"/>
+      <c r="BB47" s="114"/>
     </row>
     <row r="48" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18">
@@ -37338,10 +37346,10 @@
         <f>MAX(AT44:AT47)-MIN(AT44:AT47)+1</f>
         <v>1</v>
       </c>
-      <c r="AY48" s="140"/>
-      <c r="AZ48" s="141"/>
-      <c r="BA48" s="141"/>
-      <c r="BB48" s="142"/>
+      <c r="AY48" s="112"/>
+      <c r="AZ48" s="113"/>
+      <c r="BA48" s="113"/>
+      <c r="BB48" s="114"/>
     </row>
     <row r="49" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18">
@@ -37409,10 +37417,10 @@
         <f>MIN(AI44:AI47)</f>
         <v>-8</v>
       </c>
-      <c r="AY49" s="140"/>
-      <c r="AZ49" s="141"/>
-      <c r="BA49" s="141"/>
-      <c r="BB49" s="142"/>
+      <c r="AY49" s="112"/>
+      <c r="AZ49" s="113"/>
+      <c r="BA49" s="113"/>
+      <c r="BB49" s="114"/>
     </row>
     <row r="50" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="18">
@@ -37580,10 +37588,10 @@
         <f>AR50-AS50</f>
         <v>0</v>
       </c>
-      <c r="AY50" s="140"/>
-      <c r="AZ50" s="141"/>
-      <c r="BA50" s="141"/>
-      <c r="BB50" s="142"/>
+      <c r="AY50" s="112"/>
+      <c r="AZ50" s="113"/>
+      <c r="BA50" s="113"/>
+      <c r="BB50" s="114"/>
     </row>
     <row r="51" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="18">
@@ -37751,10 +37759,10 @@
         <f>AR51-AS51</f>
         <v>0</v>
       </c>
-      <c r="AY51" s="140"/>
-      <c r="AZ51" s="141"/>
-      <c r="BA51" s="141"/>
-      <c r="BB51" s="142"/>
+      <c r="AY51" s="112"/>
+      <c r="AZ51" s="113"/>
+      <c r="BA51" s="113"/>
+      <c r="BB51" s="114"/>
     </row>
     <row r="52" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18">
@@ -37918,10 +37926,10 @@
         <f>AR52-AS52</f>
         <v>0</v>
       </c>
-      <c r="AY52" s="143"/>
-      <c r="AZ52" s="144"/>
-      <c r="BA52" s="144"/>
-      <c r="BB52" s="145"/>
+      <c r="AY52" s="115"/>
+      <c r="AZ52" s="116"/>
+      <c r="BA52" s="116"/>
+      <c r="BB52" s="117"/>
     </row>
     <row r="53" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18">
@@ -38510,6 +38518,27 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="hexNDhodxxdoIYhe+LOVPFyB2v0aJLQphXCm5lZGwHDaP2ZITl3Lpck5mriyKWgCt8wrzYbwlizwv7dyeeElyw==" saltValue="swcCixFXOL0FnpwQehLBng==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="28">
+    <mergeCell ref="BQ6:BT7"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="A5:H6"/>
+    <mergeCell ref="J5:P6"/>
+    <mergeCell ref="AY10:AY11"/>
+    <mergeCell ref="BE12:BE13"/>
+    <mergeCell ref="AY6:BB7"/>
+    <mergeCell ref="BE6:BH7"/>
+    <mergeCell ref="BK6:BN7"/>
+    <mergeCell ref="AY22:AY23"/>
+    <mergeCell ref="BQ23:BQ24"/>
+    <mergeCell ref="AY18:AY19"/>
+    <mergeCell ref="BE20:BE21"/>
+    <mergeCell ref="AY14:AY15"/>
+    <mergeCell ref="BK16:BK17"/>
+    <mergeCell ref="AY30:AY31"/>
+    <mergeCell ref="BQ31:BT32"/>
+    <mergeCell ref="BK32:BK33"/>
+    <mergeCell ref="AY26:AY27"/>
+    <mergeCell ref="BE28:BE29"/>
     <mergeCell ref="AY46:BB52"/>
     <mergeCell ref="AY38:AY39"/>
     <mergeCell ref="BJ41:BN42"/>
@@ -38517,27 +38546,6 @@
     <mergeCell ref="BQ35:BQ36"/>
     <mergeCell ref="BE36:BE37"/>
     <mergeCell ref="BO41:BT42"/>
-    <mergeCell ref="AY30:AY31"/>
-    <mergeCell ref="BQ31:BT32"/>
-    <mergeCell ref="BK32:BK33"/>
-    <mergeCell ref="AY26:AY27"/>
-    <mergeCell ref="BE28:BE29"/>
-    <mergeCell ref="AY22:AY23"/>
-    <mergeCell ref="BQ23:BQ24"/>
-    <mergeCell ref="AY18:AY19"/>
-    <mergeCell ref="BE20:BE21"/>
-    <mergeCell ref="AY14:AY15"/>
-    <mergeCell ref="BK16:BK17"/>
-    <mergeCell ref="AY10:AY11"/>
-    <mergeCell ref="BE12:BE13"/>
-    <mergeCell ref="AY6:BB7"/>
-    <mergeCell ref="BE6:BH7"/>
-    <mergeCell ref="BK6:BN7"/>
-    <mergeCell ref="BQ6:BT7"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="A5:H6"/>
-    <mergeCell ref="J5:P6"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="F7:F55">

</xml_diff>

<commit_message>
Update results and modify checking None
</commit_message>
<xml_diff>
--- a/input/world_cup_2018_final.xlsx
+++ b/input/world_cup_2018_final.xlsx
@@ -9316,90 +9316,6 @@
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -9478,6 +9394,90 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -29897,7 +29897,7 @@
   <dimension ref="A1:BT97"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -29952,25 +29952,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:72" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="136" t="str">
+      <c r="A1" s="115" t="str">
         <f>INDEX(T,2,lang)</f>
         <v>2018 World Cup Final Tournament Schedule</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
-      <c r="J1" s="136"/>
-      <c r="K1" s="136"/>
-      <c r="L1" s="136"/>
-      <c r="M1" s="136"/>
-      <c r="N1" s="136"/>
-      <c r="O1" s="136"/>
-      <c r="P1" s="136"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
       <c r="S1" s="58"/>
       <c r="T1" s="58"/>
       <c r="U1" s="58"/>
@@ -30033,11 +30033,11 @@
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
-      <c r="O3" s="137" t="str">
+      <c r="O3" s="116" t="str">
         <f>"Language: " &amp; Settings!C4</f>
         <v>Language: English</v>
       </c>
-      <c r="P3" s="137"/>
+      <c r="P3" s="116"/>
       <c r="S3" s="58"/>
       <c r="T3" s="58"/>
       <c r="U3" s="58"/>
@@ -30063,43 +30063,43 @@
     </row>
     <row r="4" spans="1:72" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="138" t="str">
+      <c r="A5" s="117" t="str">
         <f>INDEX(T,3,lang)</f>
         <v>Group Stage</v>
       </c>
-      <c r="B5" s="139"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="140"/>
-      <c r="J5" s="144" t="s">
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="119"/>
+      <c r="J5" s="123" t="s">
         <v>2174</v>
       </c>
-      <c r="K5" s="145"/>
-      <c r="L5" s="145"/>
-      <c r="M5" s="145"/>
-      <c r="N5" s="145"/>
-      <c r="O5" s="145"/>
-      <c r="P5" s="146"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="124"/>
+      <c r="M5" s="124"/>
+      <c r="N5" s="124"/>
+      <c r="O5" s="124"/>
+      <c r="P5" s="125"/>
     </row>
     <row r="6" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="141"/>
-      <c r="B6" s="142"/>
-      <c r="C6" s="142"/>
-      <c r="D6" s="142"/>
-      <c r="E6" s="142"/>
-      <c r="F6" s="142"/>
-      <c r="G6" s="142"/>
-      <c r="H6" s="143"/>
-      <c r="J6" s="147"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="148"/>
-      <c r="M6" s="148"/>
-      <c r="N6" s="148"/>
-      <c r="O6" s="148"/>
-      <c r="P6" s="149"/>
+      <c r="A6" s="120"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="122"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="127"/>
+      <c r="N6" s="127"/>
+      <c r="O6" s="127"/>
+      <c r="P6" s="128"/>
       <c r="R6" s="58" t="s">
         <v>2175</v>
       </c>
@@ -30163,34 +30163,34 @@
       <c r="AT6" s="62" t="s">
         <v>2182</v>
       </c>
-      <c r="AY6" s="130" t="str">
+      <c r="AY6" s="109" t="str">
         <f>INDEX(T,4,lang)</f>
         <v>Round of 16</v>
       </c>
-      <c r="AZ6" s="131"/>
-      <c r="BA6" s="131"/>
-      <c r="BB6" s="132"/>
-      <c r="BE6" s="130" t="str">
+      <c r="AZ6" s="110"/>
+      <c r="BA6" s="110"/>
+      <c r="BB6" s="111"/>
+      <c r="BE6" s="109" t="str">
         <f>INDEX(T,5,lang)</f>
         <v>Quarterfinals</v>
       </c>
-      <c r="BF6" s="131"/>
-      <c r="BG6" s="131"/>
-      <c r="BH6" s="132"/>
-      <c r="BK6" s="130" t="str">
+      <c r="BF6" s="110"/>
+      <c r="BG6" s="110"/>
+      <c r="BH6" s="111"/>
+      <c r="BK6" s="109" t="str">
         <f>INDEX(T,6,lang)</f>
         <v>Semi-Finals</v>
       </c>
-      <c r="BL6" s="131"/>
-      <c r="BM6" s="131"/>
-      <c r="BN6" s="132"/>
-      <c r="BQ6" s="130" t="str">
+      <c r="BL6" s="110"/>
+      <c r="BM6" s="110"/>
+      <c r="BN6" s="111"/>
+      <c r="BQ6" s="109" t="str">
         <f>INDEX(T,8,lang)</f>
         <v>Final</v>
       </c>
-      <c r="BR6" s="131"/>
-      <c r="BS6" s="131"/>
-      <c r="BT6" s="132"/>
+      <c r="BR6" s="110"/>
+      <c r="BS6" s="110"/>
+      <c r="BT6" s="111"/>
     </row>
     <row r="7" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
@@ -30254,22 +30254,22 @@
         <f>IF(OR(F7="",G7=""),"",IF(F7&gt;G7,1,IF(F7&lt;G7,-1,0)))</f>
         <v>1</v>
       </c>
-      <c r="AY7" s="133"/>
-      <c r="AZ7" s="134"/>
-      <c r="BA7" s="134"/>
-      <c r="BB7" s="135"/>
-      <c r="BE7" s="133"/>
-      <c r="BF7" s="134"/>
-      <c r="BG7" s="134"/>
-      <c r="BH7" s="135"/>
-      <c r="BK7" s="133"/>
-      <c r="BL7" s="134"/>
-      <c r="BM7" s="134"/>
-      <c r="BN7" s="135"/>
-      <c r="BQ7" s="133"/>
-      <c r="BR7" s="134"/>
-      <c r="BS7" s="134"/>
-      <c r="BT7" s="135"/>
+      <c r="AY7" s="112"/>
+      <c r="AZ7" s="113"/>
+      <c r="BA7" s="113"/>
+      <c r="BB7" s="114"/>
+      <c r="BE7" s="112"/>
+      <c r="BF7" s="113"/>
+      <c r="BG7" s="113"/>
+      <c r="BH7" s="114"/>
+      <c r="BK7" s="112"/>
+      <c r="BL7" s="113"/>
+      <c r="BM7" s="113"/>
+      <c r="BN7" s="114"/>
+      <c r="BQ7" s="112"/>
+      <c r="BR7" s="113"/>
+      <c r="BS7" s="113"/>
+      <c r="BT7" s="114"/>
     </row>
     <row r="8" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
@@ -30525,15 +30525,15 @@
       </c>
       <c r="U9" s="59">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V9" s="58">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W9" s="58">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X9" s="58">
         <f t="shared" si="7"/>
@@ -30815,7 +30815,7 @@
         <f>AR10-AS10</f>
         <v>0</v>
       </c>
-      <c r="AY10" s="118">
+      <c r="AY10" s="129">
         <v>49</v>
       </c>
       <c r="AZ10" s="28" t="str">
@@ -31009,10 +31009,10 @@
         <f>AR11-AS11</f>
         <v>0</v>
       </c>
-      <c r="AY11" s="119"/>
+      <c r="AY11" s="130"/>
       <c r="AZ11" s="31" t="str">
         <f>AO15</f>
-        <v>2B</v>
+        <v>Portugal</v>
       </c>
       <c r="BA11" s="32"/>
       <c r="BB11" s="33"/>
@@ -31190,7 +31190,7 @@
       <c r="BB12" s="25"/>
       <c r="BC12" s="36"/>
       <c r="BD12" s="25"/>
-      <c r="BE12" s="118">
+      <c r="BE12" s="129">
         <v>57</v>
       </c>
       <c r="BF12" s="28" t="str">
@@ -31298,7 +31298,7 @@
       <c r="BB13" s="35"/>
       <c r="BC13" s="36"/>
       <c r="BD13" s="39"/>
-      <c r="BE13" s="119"/>
+      <c r="BE13" s="130"/>
       <c r="BF13" s="31" t="str">
         <f>T59</f>
         <v>W50</v>
@@ -31410,7 +31410,7 @@
       </c>
       <c r="AA14" s="58">
         <f>COUNTIF(AN14:AN17,CONCATENATE("&gt;=",AN14))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB14" s="59" t="str">
         <f>VLOOKUP("Portugal",T,lang,FALSE)</f>
@@ -31422,7 +31422,7 @@
       </c>
       <c r="AD14" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB14 &amp; "_draw")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE14" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB14 &amp; "_lose")</f>
@@ -31430,15 +31430,15 @@
       </c>
       <c r="AF14" s="58">
         <f>SUMIF($E$7:$E$54,$AB14,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB14,$G$7:$G$54)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG14" s="58">
         <f>SUMIF($E$7:$E$54,$AB14,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB14,$F$7:$F$54)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH14" s="58">
         <f>(AF14-AG14)*100+AK14*10000+AF14</f>
-        <v>40104</v>
+        <v>50105</v>
       </c>
       <c r="AI14" s="58">
         <f>AF14-AG14</f>
@@ -31450,11 +31450,11 @@
       </c>
       <c r="AK14" s="58">
         <f>AC14*3+AD14</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL14" s="58">
         <f>AP14/AP18*1000+AQ14/AQ18*100+AT14/AT18*10+AR14/AR18</f>
-        <v>50.75</v>
+        <v>0</v>
       </c>
       <c r="AM14" s="58">
         <f>VLOOKUP(AB14,db_fifarank,2,FALSE)/2000000</f>
@@ -31462,11 +31462,11 @@
       </c>
       <c r="AN14" s="59">
         <f>1000*AK14/AK18+100*AJ14+10*AF14/AF18+1*AL14/AL18+AM14</f>
-        <v>883.98135532850245</v>
+        <v>1085.000679</v>
       </c>
       <c r="AO14" s="60" t="str">
         <f>IF(SUM(AC14:AE17)=12,J15,INDEX(T,72,lang))</f>
-        <v>1B</v>
+        <v>Spain</v>
       </c>
       <c r="AP14" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB14&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB14&amp;"_win")*($U$7:$U$54))</f>
@@ -31474,21 +31474,21 @@
       </c>
       <c r="AQ14" s="62">
         <f>SUMPRODUCT(($S$7:$S$54=AB14&amp;"_draw")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB14&amp;"_draw")*($U$7:$U$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR14" s="62">
         <f>SUMPRODUCT(($E$7:$E$54=AB14)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB14)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AS14" s="62">
         <f>SUMPRODUCT(($E$7:$E$54=AB14)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB14)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AT14" s="62">
         <f>AR14-AS14</f>
         <v>0</v>
       </c>
-      <c r="AY14" s="118">
+      <c r="AY14" s="129">
         <v>50</v>
       </c>
       <c r="AZ14" s="28" t="str">
@@ -31548,11 +31548,11 @@
       </c>
       <c r="J15" s="69" t="str">
         <f>VLOOKUP(1,AA14:AK17,2,FALSE)</f>
-        <v>Portugal</v>
+        <v>Spain</v>
       </c>
       <c r="K15" s="70">
         <f>L15+M15+N15</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L15" s="70">
         <f>VLOOKUP(1,AA14:AK17,3,FALSE)</f>
@@ -31560,7 +31560,7 @@
       </c>
       <c r="M15" s="70">
         <f>VLOOKUP(1,AA14:AK17,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15" s="70">
         <f>VLOOKUP(1,AA14:AK17,5,FALSE)</f>
@@ -31568,11 +31568,11 @@
       </c>
       <c r="O15" s="70" t="str">
         <f>VLOOKUP(1,AA14:AK17,6,FALSE) &amp; " - " &amp; VLOOKUP(1,AA14:AK17,7,FALSE)</f>
-        <v>4 - 3</v>
+        <v>6 - 5</v>
       </c>
       <c r="P15" s="71">
         <f>L15*3+M15</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R15" s="58">
         <f>DATE(2018,6,17)+TIME(7,0,0)+gmt_delta</f>
@@ -31608,7 +31608,7 @@
       </c>
       <c r="AA15" s="58">
         <f>COUNTIF(AN14:AN17,CONCATENATE("&gt;=",AN15))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB15" s="59" t="str">
         <f>VLOOKUP("Spain",T,lang,FALSE)</f>
@@ -31620,7 +31620,7 @@
       </c>
       <c r="AD15" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB15 &amp; "_draw")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE15" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB15 &amp; "_lose")</f>
@@ -31628,15 +31628,15 @@
       </c>
       <c r="AF15" s="58">
         <f>SUMIF($E$7:$E$54,$AB15,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB15,$G$7:$G$54)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AG15" s="58">
         <f>SUMIF($E$7:$E$54,$AB15,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB15,$F$7:$F$54)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AH15" s="58">
         <f>(AF15-AG15)*100+AK15*10000+AF15</f>
-        <v>40104</v>
+        <v>50106</v>
       </c>
       <c r="AI15" s="58">
         <f>AF15-AG15</f>
@@ -31648,11 +31648,11 @@
       </c>
       <c r="AK15" s="58">
         <f>AC15*3+AD15</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL15" s="58">
         <f>AP15/AP18*1000+AQ15/AQ18*100+AT15/AT18*10+AR15/AR18</f>
-        <v>50.75</v>
+        <v>0</v>
       </c>
       <c r="AM15" s="58">
         <f>VLOOKUP(AB15,db_fifarank,2,FALSE)/2000000</f>
@@ -31660,11 +31660,11 @@
       </c>
       <c r="AN15" s="59">
         <f>1000*AK15/AK18+100*AJ15+10*AF15/AF18+1*AL15/AL18+AM15</f>
-        <v>883.98129182850244</v>
+        <v>1087.0006155000001</v>
       </c>
       <c r="AO15" s="60" t="str">
         <f>IF(SUM(AC14:AE17)=12,J16,INDEX(T,73,lang))</f>
-        <v>2B</v>
+        <v>Portugal</v>
       </c>
       <c r="AP15" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB15&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB15&amp;"_win")*($U$7:$U$54))</f>
@@ -31672,21 +31672,21 @@
       </c>
       <c r="AQ15" s="62">
         <f>SUMPRODUCT(($S$7:$S$54=AB15&amp;"_draw")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB15&amp;"_draw")*($U$7:$U$54))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR15" s="62">
         <f>SUMPRODUCT(($E$7:$E$54=AB15)*($U$7:$U$54)*($F$7:$F$54))+SUMPRODUCT(($H$7:$H$54=AB15)*($U$7:$U$54)*($G$7:$G$54))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AS15" s="62">
         <f>SUMPRODUCT(($E$7:$E$54=AB15)*($U$7:$U$54)*($G$7:$G$54))+SUMPRODUCT(($H$7:$H$54=AB15)*($U$7:$U$54)*($F$7:$F$54))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AT15" s="62">
         <f>AR15-AS15</f>
         <v>0</v>
       </c>
-      <c r="AY15" s="119"/>
+      <c r="AY15" s="130"/>
       <c r="AZ15" s="31" t="str">
         <f>AO27</f>
         <v>2D</v>
@@ -31747,11 +31747,11 @@
       </c>
       <c r="J16" s="72" t="str">
         <f>VLOOKUP(2,AA14:AK17,2,FALSE)</f>
-        <v>Spain</v>
+        <v>Portugal</v>
       </c>
       <c r="K16" s="27">
         <f>L16+M16+N16</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L16" s="27">
         <f>VLOOKUP(2,AA14:AK17,3,FALSE)</f>
@@ -31759,7 +31759,7 @@
       </c>
       <c r="M16" s="27">
         <f>VLOOKUP(2,AA14:AK17,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N16" s="27">
         <f>VLOOKUP(2,AA14:AK17,5,FALSE)</f>
@@ -31767,11 +31767,11 @@
       </c>
       <c r="O16" s="27" t="str">
         <f>VLOOKUP(2,AA14:AK17,6,FALSE) &amp; " - " &amp; VLOOKUP(2,AA14:AK17,7,FALSE)</f>
-        <v>4 - 3</v>
+        <v>5 - 4</v>
       </c>
       <c r="P16" s="73">
         <f>L16*3+M16</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R16" s="58">
         <f>DATE(2018,6,17)+TIME(1,0,0)+gmt_delta</f>
@@ -31819,7 +31819,7 @@
       </c>
       <c r="AD16" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB16 &amp; "_draw")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE16" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB16 &amp; "_lose")</f>
@@ -31827,15 +31827,15 @@
       </c>
       <c r="AF16" s="58">
         <f>SUMIF($E$7:$E$54,$AB16,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB16,$G$7:$G$54)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG16" s="58">
         <f>SUMIF($E$7:$E$54,$AB16,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB16,$F$7:$F$54)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AH16" s="58">
         <f>(AF16-AG16)*100+AK16*10000+AF16</f>
-        <v>-200</v>
+        <v>9802</v>
       </c>
       <c r="AI16" s="58">
         <f>AF16-AG16</f>
@@ -31847,7 +31847,7 @@
       </c>
       <c r="AK16" s="58">
         <f>AC16*3+AD16</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL16" s="58">
         <f>AP16/AP18*1000+AQ16/AQ18*100+AT16/AT18*10+AR16/AR18</f>
@@ -31859,7 +31859,7 @@
       </c>
       <c r="AN16" s="59">
         <f>1000*AK16/AK18+100*AJ16+10*AF16/AF18+1*AL16/AL18+AM16</f>
-        <v>3.6900000000000002E-4</v>
+        <v>204.00036900000001</v>
       </c>
       <c r="AP16" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB16&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB16&amp;"_win")*($U$7:$U$54))</f>
@@ -31893,7 +31893,7 @@
       <c r="BH16" s="25"/>
       <c r="BI16" s="36"/>
       <c r="BJ16" s="25"/>
-      <c r="BK16" s="118">
+      <c r="BK16" s="129">
         <v>61</v>
       </c>
       <c r="BL16" s="28" t="str">
@@ -31945,7 +31945,7 @@
       </c>
       <c r="K17" s="27">
         <f>L17+M17+N17</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L17" s="27">
         <f>VLOOKUP(3,AA14:AK17,3,FALSE)</f>
@@ -31953,7 +31953,7 @@
       </c>
       <c r="M17" s="27">
         <f>VLOOKUP(3,AA14:AK17,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" s="27">
         <f>VLOOKUP(3,AA14:AK17,5,FALSE)</f>
@@ -31961,11 +31961,11 @@
       </c>
       <c r="O17" s="27" t="str">
         <f>VLOOKUP(3,AA14:AK17,6,FALSE) &amp; " - " &amp; VLOOKUP(3,AA14:AK17,7,FALSE)</f>
-        <v>1 - 1</v>
+        <v>2 - 2</v>
       </c>
       <c r="P17" s="73">
         <f>L17*3+M17</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R17" s="58">
         <f>DATE(2018,6,17)+TIME(4,0,0)+gmt_delta</f>
@@ -32013,7 +32013,7 @@
       </c>
       <c r="AD17" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB17 &amp; "_draw")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE17" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB17 &amp; "_lose")</f>
@@ -32021,15 +32021,15 @@
       </c>
       <c r="AF17" s="58">
         <f>SUMIF($E$7:$E$54,$AB17,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB17,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG17" s="58">
         <f>SUMIF($E$7:$E$54,$AB17,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB17,$F$7:$F$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH17" s="58">
         <f>(AF17-AG17)*100+AK17*10000+AF17</f>
-        <v>30001</v>
+        <v>40002</v>
       </c>
       <c r="AI17" s="58">
         <f>AF17-AG17</f>
@@ -32041,7 +32041,7 @@
       </c>
       <c r="AK17" s="58">
         <f>AC17*3+AD17</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL17" s="58">
         <f>AP17/AP18*1000+AQ17/AQ18*100+AT17/AT18*10+AR17/AR18</f>
@@ -32053,7 +32053,7 @@
       </c>
       <c r="AN17" s="59">
         <f>1000*AK17/AK18+100*AJ17+10*AF17/AF18+1*AL17/AL18+AM17</f>
-        <v>652.00039900000002</v>
+        <v>854.00039900000002</v>
       </c>
       <c r="AP17" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB17&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB17&amp;"_win")*($U$7:$U$54))</f>
@@ -32090,7 +32090,7 @@
       <c r="BH17" s="25"/>
       <c r="BI17" s="36"/>
       <c r="BJ17" s="39"/>
-      <c r="BK17" s="119"/>
+      <c r="BK17" s="130"/>
       <c r="BL17" s="31" t="str">
         <f>T70</f>
         <v>W58</v>
@@ -32140,7 +32140,7 @@
       </c>
       <c r="K18" s="75">
         <f>L18+M18+N18</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L18" s="75">
         <f>VLOOKUP(4,AA14:AK17,3,FALSE)</f>
@@ -32148,7 +32148,7 @@
       </c>
       <c r="M18" s="75">
         <f>VLOOKUP(4,AA14:AK17,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="75">
         <f>VLOOKUP(4,AA14:AK17,5,FALSE)</f>
@@ -32156,11 +32156,11 @@
       </c>
       <c r="O18" s="75" t="str">
         <f>VLOOKUP(4,AA14:AK17,6,FALSE) &amp; " - " &amp; VLOOKUP(4,AA14:AK17,7,FALSE)</f>
-        <v>0 - 2</v>
+        <v>2 - 4</v>
       </c>
       <c r="P18" s="76">
         <f>L18*3+M18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R18" s="58">
         <f>DATE(2018,6,18)+TIME(1,0,0)+gmt_delta</f>
@@ -32212,7 +32212,7 @@
       </c>
       <c r="AG18" s="58">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH18" s="58">
         <f>MAX(AH14:AH17)-AH19+1</f>
@@ -32228,7 +32228,7 @@
       </c>
       <c r="AL18" s="58">
         <f t="shared" si="11"/>
-        <v>51.75</v>
+        <v>1</v>
       </c>
       <c r="AP18" s="58">
         <f>MAX(AP14:AP17)-MIN(AP14:AP17)+1</f>
@@ -32236,21 +32236,21 @@
       </c>
       <c r="AQ18" s="58">
         <f>MAX(AQ14:AQ17)-MIN(AQ14:AQ17)+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AR18" s="58">
         <f>MAX(AR14:AR17)-MIN(AR14:AR17)+1</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AS18" s="58">
         <f>MAX(AS14:AS17)-MIN(AS14:AS17)+1</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AT18" s="58">
         <f>MAX(AT14:AT17)-MIN(AT14:AT17)+1</f>
         <v>1</v>
       </c>
-      <c r="AY18" s="118">
+      <c r="AY18" s="129">
         <v>53</v>
       </c>
       <c r="AZ18" s="28" t="str">
@@ -32349,13 +32349,13 @@
       </c>
       <c r="AH19" s="58">
         <f>MIN(AH14:AH17)</f>
-        <v>-200</v>
+        <v>9802</v>
       </c>
       <c r="AI19" s="58">
         <f>MIN(AI14:AI17)</f>
         <v>-2</v>
       </c>
-      <c r="AY19" s="119"/>
+      <c r="AY19" s="130"/>
       <c r="AZ19" s="31" t="str">
         <f>AO39</f>
         <v>2F</v>
@@ -32560,7 +32560,7 @@
       <c r="BB20" s="25"/>
       <c r="BC20" s="36"/>
       <c r="BD20" s="25"/>
-      <c r="BE20" s="118">
+      <c r="BE20" s="129">
         <v>58</v>
       </c>
       <c r="BF20" s="28" t="str">
@@ -32761,7 +32761,7 @@
       <c r="BB21" s="35"/>
       <c r="BC21" s="36"/>
       <c r="BD21" s="39"/>
-      <c r="BE21" s="119"/>
+      <c r="BE21" s="130"/>
       <c r="BF21" s="31" t="str">
         <f>T63</f>
         <v>W54</v>
@@ -32947,7 +32947,7 @@
         <f>AR22-AS22</f>
         <v>0</v>
       </c>
-      <c r="AY22" s="118">
+      <c r="AY22" s="129">
         <v>54</v>
       </c>
       <c r="AZ22" s="28" t="str">
@@ -33144,7 +33144,7 @@
         <f>AR23-AS23</f>
         <v>0</v>
       </c>
-      <c r="AY23" s="119"/>
+      <c r="AY23" s="130"/>
       <c r="AZ23" s="31" t="str">
         <f>AO51</f>
         <v>2H</v>
@@ -33165,7 +33165,7 @@
       <c r="BN23" s="25"/>
       <c r="BO23" s="36"/>
       <c r="BP23" s="25"/>
-      <c r="BQ23" s="118">
+      <c r="BQ23" s="129">
         <v>64</v>
       </c>
       <c r="BR23" s="28" t="str">
@@ -33338,7 +33338,7 @@
       <c r="BN24" s="25"/>
       <c r="BO24" s="36"/>
       <c r="BP24" s="39"/>
-      <c r="BQ24" s="119"/>
+      <c r="BQ24" s="130"/>
       <c r="BR24" s="31" t="str">
         <f>T77</f>
         <v>W62</v>
@@ -33619,12 +33619,12 @@
         <f>AR26-AS26</f>
         <v>0</v>
       </c>
-      <c r="AY26" s="118">
+      <c r="AY26" s="129">
         <v>51</v>
       </c>
       <c r="AZ26" s="28" t="str">
         <f>AO14</f>
-        <v>1B</v>
+        <v>Spain</v>
       </c>
       <c r="BA26" s="29"/>
       <c r="BB26" s="30"/>
@@ -33817,7 +33817,7 @@
         <f>AR27-AS27</f>
         <v>0</v>
       </c>
-      <c r="AY27" s="119"/>
+      <c r="AY27" s="130"/>
       <c r="AZ27" s="31" t="str">
         <f>AO9</f>
         <v>Russia</v>
@@ -34018,7 +34018,7 @@
       <c r="BB28" s="25"/>
       <c r="BC28" s="36"/>
       <c r="BD28" s="25"/>
-      <c r="BE28" s="118">
+      <c r="BE28" s="129">
         <v>59</v>
       </c>
       <c r="BF28" s="28" t="str">
@@ -34215,7 +34215,7 @@
       <c r="BB29" s="35"/>
       <c r="BC29" s="36"/>
       <c r="BD29" s="39"/>
-      <c r="BE29" s="119"/>
+      <c r="BE29" s="130"/>
       <c r="BF29" s="31" t="str">
         <f>T61</f>
         <v>W52</v>
@@ -34381,7 +34381,7 @@
         <f>MAX(AT26:AT29)-MIN(AT26:AT29)+1</f>
         <v>1</v>
       </c>
-      <c r="AY30" s="118">
+      <c r="AY30" s="129">
         <v>52</v>
       </c>
       <c r="AZ30" s="28" t="str">
@@ -34479,7 +34479,7 @@
         <f>MIN(AI26:AI29)</f>
         <v>-3</v>
       </c>
-      <c r="AY31" s="119"/>
+      <c r="AY31" s="130"/>
       <c r="AZ31" s="31" t="str">
         <f>AO21</f>
         <v>2C</v>
@@ -34503,13 +34503,13 @@
       <c r="BN31" s="35"/>
       <c r="BO31" s="36"/>
       <c r="BP31" s="41"/>
-      <c r="BQ31" s="124" t="str">
+      <c r="BQ31" s="131" t="str">
         <f>INDEX(T,7,lang)</f>
         <v>Third-Place Play-Off</v>
       </c>
-      <c r="BR31" s="125"/>
-      <c r="BS31" s="125"/>
-      <c r="BT31" s="126"/>
+      <c r="BR31" s="132"/>
+      <c r="BS31" s="132"/>
+      <c r="BT31" s="133"/>
     </row>
     <row r="32" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18">
@@ -34693,7 +34693,7 @@
       <c r="BH32" s="25"/>
       <c r="BI32" s="36"/>
       <c r="BJ32" s="25"/>
-      <c r="BK32" s="118">
+      <c r="BK32" s="129">
         <v>62</v>
       </c>
       <c r="BL32" s="28" t="str">
@@ -34704,10 +34704,10 @@
       <c r="BN32" s="30"/>
       <c r="BO32" s="40"/>
       <c r="BP32" s="41"/>
-      <c r="BQ32" s="127"/>
-      <c r="BR32" s="128"/>
-      <c r="BS32" s="128"/>
-      <c r="BT32" s="129"/>
+      <c r="BQ32" s="134"/>
+      <c r="BR32" s="135"/>
+      <c r="BS32" s="135"/>
+      <c r="BT32" s="136"/>
     </row>
     <row r="33" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
@@ -34894,7 +34894,7 @@
       <c r="BH33" s="25"/>
       <c r="BI33" s="36"/>
       <c r="BJ33" s="39"/>
-      <c r="BK33" s="119"/>
+      <c r="BK33" s="130"/>
       <c r="BL33" s="31" t="str">
         <f>T72</f>
         <v>W60</v>
@@ -35074,7 +35074,7 @@
         <f>AR34-AS34</f>
         <v>0</v>
       </c>
-      <c r="AY34" s="118">
+      <c r="AY34" s="129">
         <v>55</v>
       </c>
       <c r="AZ34" s="28" t="str">
@@ -35271,7 +35271,7 @@
         <f>AR35-AS35</f>
         <v>0</v>
       </c>
-      <c r="AY35" s="119"/>
+      <c r="AY35" s="130"/>
       <c r="AZ35" s="31" t="str">
         <f>AO33</f>
         <v>2E</v>
@@ -35295,7 +35295,7 @@
       <c r="BN35" s="25"/>
       <c r="BO35" s="25"/>
       <c r="BP35" s="25"/>
-      <c r="BQ35" s="118">
+      <c r="BQ35" s="129">
         <v>63</v>
       </c>
       <c r="BR35" s="28" t="str">
@@ -35457,7 +35457,7 @@
       <c r="BB36" s="25"/>
       <c r="BC36" s="36"/>
       <c r="BD36" s="25"/>
-      <c r="BE36" s="118">
+      <c r="BE36" s="129">
         <v>60</v>
       </c>
       <c r="BF36" s="28" t="str">
@@ -35474,7 +35474,7 @@
       <c r="BN36" s="25"/>
       <c r="BO36" s="25"/>
       <c r="BP36" s="25"/>
-      <c r="BQ36" s="119"/>
+      <c r="BQ36" s="130"/>
       <c r="BR36" s="31" t="str">
         <f>Z77</f>
         <v>L62</v>
@@ -35561,7 +35561,7 @@
       <c r="BB37" s="35"/>
       <c r="BC37" s="36"/>
       <c r="BD37" s="39"/>
-      <c r="BE37" s="119"/>
+      <c r="BE37" s="130"/>
       <c r="BF37" s="31" t="str">
         <f>T65</f>
         <v>W56</v>
@@ -35751,7 +35751,7 @@
         <f>AR38-AS38</f>
         <v>1</v>
       </c>
-      <c r="AY38" s="118">
+      <c r="AY38" s="129">
         <v>56</v>
       </c>
       <c r="AZ38" s="28" t="str">
@@ -35945,7 +35945,7 @@
         <f>AR39-AS39</f>
         <v>0</v>
       </c>
-      <c r="AY39" s="119"/>
+      <c r="AY39" s="130"/>
       <c r="AZ39" s="31" t="str">
         <f>AO45</f>
         <v>2G</v>
@@ -36152,8 +36152,12 @@
         <f>AB17</f>
         <v>Iran</v>
       </c>
-      <c r="F41" s="23"/>
-      <c r="G41" s="24"/>
+      <c r="F41" s="23">
+        <v>1</v>
+      </c>
+      <c r="G41" s="24">
+        <v>1</v>
+      </c>
       <c r="H41" s="67" t="str">
         <f>AB14</f>
         <v>Portugal</v>
@@ -36192,11 +36196,11 @@
       </c>
       <c r="S41" s="65" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Iran_draw</v>
       </c>
       <c r="T41" s="65" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Portugal_draw</v>
       </c>
       <c r="U41" s="59">
         <f t="shared" si="4"/>
@@ -36214,9 +36218,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y41" s="58" t="str">
+      <c r="Y41" s="58">
         <f t="shared" si="9"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="AA41" s="58">
         <f>COUNTIF(AN38:AN41,CONCATENATE("&gt;=",AN41))</f>
@@ -36294,23 +36298,23 @@
         <f>AR41-AS41</f>
         <v>0</v>
       </c>
-      <c r="BJ41" s="120" t="str">
+      <c r="BJ41" s="146" t="str">
         <f>INDEX(T,102,lang)</f>
         <v>World Champion 2018</v>
       </c>
-      <c r="BK41" s="120"/>
-      <c r="BL41" s="120"/>
-      <c r="BM41" s="120"/>
-      <c r="BN41" s="120"/>
-      <c r="BO41" s="122" t="str">
+      <c r="BK41" s="146"/>
+      <c r="BL41" s="146"/>
+      <c r="BM41" s="146"/>
+      <c r="BN41" s="146"/>
+      <c r="BO41" s="148" t="str">
         <f>S85</f>
         <v/>
       </c>
-      <c r="BP41" s="122"/>
-      <c r="BQ41" s="122"/>
-      <c r="BR41" s="122"/>
-      <c r="BS41" s="122"/>
-      <c r="BT41" s="122"/>
+      <c r="BP41" s="148"/>
+      <c r="BQ41" s="148"/>
+      <c r="BR41" s="148"/>
+      <c r="BS41" s="148"/>
+      <c r="BT41" s="148"/>
     </row>
     <row r="42" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18">
@@ -36332,8 +36336,12 @@
         <f>AB15</f>
         <v>Spain</v>
       </c>
-      <c r="F42" s="23"/>
-      <c r="G42" s="24"/>
+      <c r="F42" s="23">
+        <v>2</v>
+      </c>
+      <c r="G42" s="24">
+        <v>2</v>
+      </c>
       <c r="H42" s="67" t="str">
         <f>AB16</f>
         <v>Morocco</v>
@@ -36372,11 +36380,11 @@
       </c>
       <c r="S42" s="65" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Spain_draw</v>
       </c>
       <c r="T42" s="65" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Morocco_draw</v>
       </c>
       <c r="U42" s="59">
         <f t="shared" si="4"/>
@@ -36394,9 +36402,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y42" s="58" t="str">
+      <c r="Y42" s="58">
         <f t="shared" si="9"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="AC42" s="58">
         <f t="shared" ref="AC42:AL42" si="15">MAX(AC38:AC41)-MIN(AC38:AC41)+1</f>
@@ -36454,17 +36462,17 @@
         <f>MAX(AT38:AT41)-MIN(AT38:AT41)+1</f>
         <v>3</v>
       </c>
-      <c r="BJ42" s="121"/>
-      <c r="BK42" s="121"/>
-      <c r="BL42" s="121"/>
-      <c r="BM42" s="121"/>
-      <c r="BN42" s="121"/>
-      <c r="BO42" s="123"/>
-      <c r="BP42" s="123"/>
-      <c r="BQ42" s="123"/>
-      <c r="BR42" s="123"/>
-      <c r="BS42" s="123"/>
-      <c r="BT42" s="123"/>
+      <c r="BJ42" s="147"/>
+      <c r="BK42" s="147"/>
+      <c r="BL42" s="147"/>
+      <c r="BM42" s="147"/>
+      <c r="BN42" s="147"/>
+      <c r="BO42" s="149"/>
+      <c r="BP42" s="149"/>
+      <c r="BQ42" s="149"/>
+      <c r="BR42" s="149"/>
+      <c r="BS42" s="149"/>
+      <c r="BT42" s="149"/>
     </row>
     <row r="43" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18">
@@ -37030,12 +37038,12 @@
         <f>AR46-AS46</f>
         <v>0</v>
       </c>
-      <c r="AY46" s="109" t="s">
+      <c r="AY46" s="137" t="s">
         <v>2224</v>
       </c>
-      <c r="AZ46" s="110"/>
-      <c r="BA46" s="110"/>
-      <c r="BB46" s="111"/>
+      <c r="AZ46" s="138"/>
+      <c r="BA46" s="138"/>
+      <c r="BB46" s="139"/>
     </row>
     <row r="47" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18">
@@ -37199,10 +37207,10 @@
         <f>AR47-AS47</f>
         <v>0</v>
       </c>
-      <c r="AY47" s="112"/>
-      <c r="AZ47" s="113"/>
-      <c r="BA47" s="113"/>
-      <c r="BB47" s="114"/>
+      <c r="AY47" s="140"/>
+      <c r="AZ47" s="141"/>
+      <c r="BA47" s="141"/>
+      <c r="BB47" s="142"/>
     </row>
     <row r="48" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18">
@@ -37346,10 +37354,10 @@
         <f>MAX(AT44:AT47)-MIN(AT44:AT47)+1</f>
         <v>1</v>
       </c>
-      <c r="AY48" s="112"/>
-      <c r="AZ48" s="113"/>
-      <c r="BA48" s="113"/>
-      <c r="BB48" s="114"/>
+      <c r="AY48" s="140"/>
+      <c r="AZ48" s="141"/>
+      <c r="BA48" s="141"/>
+      <c r="BB48" s="142"/>
     </row>
     <row r="49" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18">
@@ -37417,10 +37425,10 @@
         <f>MIN(AI44:AI47)</f>
         <v>-8</v>
       </c>
-      <c r="AY49" s="112"/>
-      <c r="AZ49" s="113"/>
-      <c r="BA49" s="113"/>
-      <c r="BB49" s="114"/>
+      <c r="AY49" s="140"/>
+      <c r="AZ49" s="141"/>
+      <c r="BA49" s="141"/>
+      <c r="BB49" s="142"/>
     </row>
     <row r="50" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="18">
@@ -37588,10 +37596,10 @@
         <f>AR50-AS50</f>
         <v>0</v>
       </c>
-      <c r="AY50" s="112"/>
-      <c r="AZ50" s="113"/>
-      <c r="BA50" s="113"/>
-      <c r="BB50" s="114"/>
+      <c r="AY50" s="140"/>
+      <c r="AZ50" s="141"/>
+      <c r="BA50" s="141"/>
+      <c r="BB50" s="142"/>
     </row>
     <row r="51" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="18">
@@ -37759,10 +37767,10 @@
         <f>AR51-AS51</f>
         <v>0</v>
       </c>
-      <c r="AY51" s="112"/>
-      <c r="AZ51" s="113"/>
-      <c r="BA51" s="113"/>
-      <c r="BB51" s="114"/>
+      <c r="AY51" s="140"/>
+      <c r="AZ51" s="141"/>
+      <c r="BA51" s="141"/>
+      <c r="BB51" s="142"/>
     </row>
     <row r="52" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18">
@@ -37926,10 +37934,10 @@
         <f>AR52-AS52</f>
         <v>0</v>
       </c>
-      <c r="AY52" s="115"/>
-      <c r="AZ52" s="116"/>
-      <c r="BA52" s="116"/>
-      <c r="BB52" s="117"/>
+      <c r="AY52" s="143"/>
+      <c r="AZ52" s="144"/>
+      <c r="BA52" s="144"/>
+      <c r="BB52" s="145"/>
     </row>
     <row r="53" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18">
@@ -38518,27 +38526,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="hexNDhodxxdoIYhe+LOVPFyB2v0aJLQphXCm5lZGwHDaP2ZITl3Lpck5mriyKWgCt8wrzYbwlizwv7dyeeElyw==" saltValue="swcCixFXOL0FnpwQehLBng==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="28">
-    <mergeCell ref="BQ6:BT7"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="A5:H6"/>
-    <mergeCell ref="J5:P6"/>
-    <mergeCell ref="AY10:AY11"/>
-    <mergeCell ref="BE12:BE13"/>
-    <mergeCell ref="AY6:BB7"/>
-    <mergeCell ref="BE6:BH7"/>
-    <mergeCell ref="BK6:BN7"/>
-    <mergeCell ref="AY22:AY23"/>
-    <mergeCell ref="BQ23:BQ24"/>
-    <mergeCell ref="AY18:AY19"/>
-    <mergeCell ref="BE20:BE21"/>
-    <mergeCell ref="AY14:AY15"/>
-    <mergeCell ref="BK16:BK17"/>
-    <mergeCell ref="AY30:AY31"/>
-    <mergeCell ref="BQ31:BT32"/>
-    <mergeCell ref="BK32:BK33"/>
-    <mergeCell ref="AY26:AY27"/>
-    <mergeCell ref="BE28:BE29"/>
     <mergeCell ref="AY46:BB52"/>
     <mergeCell ref="AY38:AY39"/>
     <mergeCell ref="BJ41:BN42"/>
@@ -38546,6 +38533,27 @@
     <mergeCell ref="BQ35:BQ36"/>
     <mergeCell ref="BE36:BE37"/>
     <mergeCell ref="BO41:BT42"/>
+    <mergeCell ref="AY30:AY31"/>
+    <mergeCell ref="BQ31:BT32"/>
+    <mergeCell ref="BK32:BK33"/>
+    <mergeCell ref="AY26:AY27"/>
+    <mergeCell ref="BE28:BE29"/>
+    <mergeCell ref="AY22:AY23"/>
+    <mergeCell ref="BQ23:BQ24"/>
+    <mergeCell ref="AY18:AY19"/>
+    <mergeCell ref="BE20:BE21"/>
+    <mergeCell ref="AY14:AY15"/>
+    <mergeCell ref="BK16:BK17"/>
+    <mergeCell ref="AY10:AY11"/>
+    <mergeCell ref="BE12:BE13"/>
+    <mergeCell ref="AY6:BB7"/>
+    <mergeCell ref="BE6:BH7"/>
+    <mergeCell ref="BK6:BN7"/>
+    <mergeCell ref="BQ6:BT7"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="A5:H6"/>
+    <mergeCell ref="J5:P6"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="F7:F55">

</xml_diff>

<commit_message>
Add linechart and update latest scores
</commit_message>
<xml_diff>
--- a/input/world_cup_2018_final.xlsx
+++ b/input/world_cup_2018_final.xlsx
@@ -9316,6 +9316,90 @@
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -9394,90 +9478,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -29897,7 +29897,7 @@
   <dimension ref="A1:BT97"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -29952,25 +29952,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:72" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="115" t="str">
+      <c r="A1" s="136" t="str">
         <f>INDEX(T,2,lang)</f>
         <v>2018 World Cup Final Tournament Schedule</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="136"/>
+      <c r="M1" s="136"/>
+      <c r="N1" s="136"/>
+      <c r="O1" s="136"/>
+      <c r="P1" s="136"/>
       <c r="S1" s="58"/>
       <c r="T1" s="58"/>
       <c r="U1" s="58"/>
@@ -30033,11 +30033,11 @@
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
-      <c r="O3" s="116" t="str">
+      <c r="O3" s="137" t="str">
         <f>"Language: " &amp; Settings!C4</f>
         <v>Language: English</v>
       </c>
-      <c r="P3" s="116"/>
+      <c r="P3" s="137"/>
       <c r="S3" s="58"/>
       <c r="T3" s="58"/>
       <c r="U3" s="58"/>
@@ -30063,43 +30063,43 @@
     </row>
     <row r="4" spans="1:72" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="117" t="str">
+      <c r="A5" s="138" t="str">
         <f>INDEX(T,3,lang)</f>
         <v>Group Stage</v>
       </c>
-      <c r="B5" s="118"/>
-      <c r="C5" s="118"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="119"/>
-      <c r="J5" s="123" t="s">
+      <c r="B5" s="139"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="139"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="140"/>
+      <c r="J5" s="144" t="s">
         <v>2174</v>
       </c>
-      <c r="K5" s="124"/>
-      <c r="L5" s="124"/>
-      <c r="M5" s="124"/>
-      <c r="N5" s="124"/>
-      <c r="O5" s="124"/>
-      <c r="P5" s="125"/>
+      <c r="K5" s="145"/>
+      <c r="L5" s="145"/>
+      <c r="M5" s="145"/>
+      <c r="N5" s="145"/>
+      <c r="O5" s="145"/>
+      <c r="P5" s="146"/>
     </row>
     <row r="6" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="120"/>
-      <c r="B6" s="121"/>
-      <c r="C6" s="121"/>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="121"/>
-      <c r="H6" s="122"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="127"/>
-      <c r="M6" s="127"/>
-      <c r="N6" s="127"/>
-      <c r="O6" s="127"/>
-      <c r="P6" s="128"/>
+      <c r="A6" s="141"/>
+      <c r="B6" s="142"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="142"/>
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="143"/>
+      <c r="J6" s="147"/>
+      <c r="K6" s="148"/>
+      <c r="L6" s="148"/>
+      <c r="M6" s="148"/>
+      <c r="N6" s="148"/>
+      <c r="O6" s="148"/>
+      <c r="P6" s="149"/>
       <c r="R6" s="58" t="s">
         <v>2175</v>
       </c>
@@ -30163,34 +30163,34 @@
       <c r="AT6" s="62" t="s">
         <v>2182</v>
       </c>
-      <c r="AY6" s="109" t="str">
+      <c r="AY6" s="130" t="str">
         <f>INDEX(T,4,lang)</f>
         <v>Round of 16</v>
       </c>
-      <c r="AZ6" s="110"/>
-      <c r="BA6" s="110"/>
-      <c r="BB6" s="111"/>
-      <c r="BE6" s="109" t="str">
+      <c r="AZ6" s="131"/>
+      <c r="BA6" s="131"/>
+      <c r="BB6" s="132"/>
+      <c r="BE6" s="130" t="str">
         <f>INDEX(T,5,lang)</f>
         <v>Quarterfinals</v>
       </c>
-      <c r="BF6" s="110"/>
-      <c r="BG6" s="110"/>
-      <c r="BH6" s="111"/>
-      <c r="BK6" s="109" t="str">
+      <c r="BF6" s="131"/>
+      <c r="BG6" s="131"/>
+      <c r="BH6" s="132"/>
+      <c r="BK6" s="130" t="str">
         <f>INDEX(T,6,lang)</f>
         <v>Semi-Finals</v>
       </c>
-      <c r="BL6" s="110"/>
-      <c r="BM6" s="110"/>
-      <c r="BN6" s="111"/>
-      <c r="BQ6" s="109" t="str">
+      <c r="BL6" s="131"/>
+      <c r="BM6" s="131"/>
+      <c r="BN6" s="132"/>
+      <c r="BQ6" s="130" t="str">
         <f>INDEX(T,8,lang)</f>
         <v>Final</v>
       </c>
-      <c r="BR6" s="110"/>
-      <c r="BS6" s="110"/>
-      <c r="BT6" s="111"/>
+      <c r="BR6" s="131"/>
+      <c r="BS6" s="131"/>
+      <c r="BT6" s="132"/>
     </row>
     <row r="7" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
@@ -30254,22 +30254,22 @@
         <f>IF(OR(F7="",G7=""),"",IF(F7&gt;G7,1,IF(F7&lt;G7,-1,0)))</f>
         <v>1</v>
       </c>
-      <c r="AY7" s="112"/>
-      <c r="AZ7" s="113"/>
-      <c r="BA7" s="113"/>
-      <c r="BB7" s="114"/>
-      <c r="BE7" s="112"/>
-      <c r="BF7" s="113"/>
-      <c r="BG7" s="113"/>
-      <c r="BH7" s="114"/>
-      <c r="BK7" s="112"/>
-      <c r="BL7" s="113"/>
-      <c r="BM7" s="113"/>
-      <c r="BN7" s="114"/>
-      <c r="BQ7" s="112"/>
-      <c r="BR7" s="113"/>
-      <c r="BS7" s="113"/>
-      <c r="BT7" s="114"/>
+      <c r="AY7" s="133"/>
+      <c r="AZ7" s="134"/>
+      <c r="BA7" s="134"/>
+      <c r="BB7" s="135"/>
+      <c r="BE7" s="133"/>
+      <c r="BF7" s="134"/>
+      <c r="BG7" s="134"/>
+      <c r="BH7" s="135"/>
+      <c r="BK7" s="133"/>
+      <c r="BL7" s="134"/>
+      <c r="BM7" s="134"/>
+      <c r="BN7" s="135"/>
+      <c r="BQ7" s="133"/>
+      <c r="BR7" s="134"/>
+      <c r="BS7" s="134"/>
+      <c r="BT7" s="135"/>
     </row>
     <row r="8" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
@@ -30815,7 +30815,7 @@
         <f>AR10-AS10</f>
         <v>0</v>
       </c>
-      <c r="AY10" s="129">
+      <c r="AY10" s="118">
         <v>49</v>
       </c>
       <c r="AZ10" s="28" t="str">
@@ -31009,7 +31009,7 @@
         <f>AR11-AS11</f>
         <v>0</v>
       </c>
-      <c r="AY11" s="130"/>
+      <c r="AY11" s="119"/>
       <c r="AZ11" s="31" t="str">
         <f>AO15</f>
         <v>Portugal</v>
@@ -31190,7 +31190,7 @@
       <c r="BB12" s="25"/>
       <c r="BC12" s="36"/>
       <c r="BD12" s="25"/>
-      <c r="BE12" s="129">
+      <c r="BE12" s="118">
         <v>57</v>
       </c>
       <c r="BF12" s="28" t="str">
@@ -31298,7 +31298,7 @@
       <c r="BB13" s="35"/>
       <c r="BC13" s="36"/>
       <c r="BD13" s="39"/>
-      <c r="BE13" s="130"/>
+      <c r="BE13" s="119"/>
       <c r="BF13" s="31" t="str">
         <f>T59</f>
         <v>W50</v>
@@ -31488,12 +31488,12 @@
         <f>AR14-AS14</f>
         <v>0</v>
       </c>
-      <c r="AY14" s="129">
+      <c r="AY14" s="118">
         <v>50</v>
       </c>
       <c r="AZ14" s="28" t="str">
         <f>AO20</f>
-        <v>1C</v>
+        <v>France</v>
       </c>
       <c r="BA14" s="29"/>
       <c r="BB14" s="30"/>
@@ -31686,7 +31686,7 @@
         <f>AR15-AS15</f>
         <v>0</v>
       </c>
-      <c r="AY15" s="130"/>
+      <c r="AY15" s="119"/>
       <c r="AZ15" s="31" t="str">
         <f>AO27</f>
         <v>2D</v>
@@ -31893,7 +31893,7 @@
       <c r="BH16" s="25"/>
       <c r="BI16" s="36"/>
       <c r="BJ16" s="25"/>
-      <c r="BK16" s="129">
+      <c r="BK16" s="118">
         <v>61</v>
       </c>
       <c r="BL16" s="28" t="str">
@@ -32090,7 +32090,7 @@
       <c r="BH17" s="25"/>
       <c r="BI17" s="36"/>
       <c r="BJ17" s="39"/>
-      <c r="BK17" s="130"/>
+      <c r="BK17" s="119"/>
       <c r="BL17" s="31" t="str">
         <f>T70</f>
         <v>W58</v>
@@ -32250,7 +32250,7 @@
         <f>MAX(AT14:AT17)-MIN(AT14:AT17)+1</f>
         <v>1</v>
       </c>
-      <c r="AY18" s="129">
+      <c r="AY18" s="118">
         <v>53</v>
       </c>
       <c r="AZ18" s="28" t="str">
@@ -32355,7 +32355,7 @@
         <f>MIN(AI14:AI17)</f>
         <v>-2</v>
       </c>
-      <c r="AY19" s="130"/>
+      <c r="AY19" s="119"/>
       <c r="AZ19" s="31" t="str">
         <f>AO39</f>
         <v>2F</v>
@@ -32488,7 +32488,7 @@
       </c>
       <c r="AD20" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB20 &amp; "_draw")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE20" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB20 &amp; "_lose")</f>
@@ -32504,7 +32504,7 @@
       </c>
       <c r="AH20" s="58">
         <f>(AF20-AG20)*100+AK20*10000+AF20</f>
-        <v>60203</v>
+        <v>70203</v>
       </c>
       <c r="AI20" s="58">
         <f>AF20-AG20</f>
@@ -32512,11 +32512,11 @@
       </c>
       <c r="AJ20" s="58">
         <f>(AI20-AI25)/AI24</f>
-        <v>0.8</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="AK20" s="58">
         <f>AC20*3+AD20</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AL20" s="58">
         <f>AP20/AP24*1000+AQ20/AQ24*100+AT20/AT24*10+AR20/AR24</f>
@@ -32528,11 +32528,11 @@
       </c>
       <c r="AN20" s="59">
         <f>1000*AK20/AK24+100*AJ20+10*AF20/AF24+1*AL20/AL24+AM20</f>
-        <v>944.64344864285715</v>
+        <v>1098.3339248333332</v>
       </c>
       <c r="AO20" s="60" t="str">
         <f>IF(SUM(AC20:AE23)=12,J21,INDEX(T,74,lang))</f>
-        <v>1C</v>
+        <v>France</v>
       </c>
       <c r="AP20" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB20&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB20&amp;"_win")*($U$7:$U$54))</f>
@@ -32560,7 +32560,7 @@
       <c r="BB20" s="25"/>
       <c r="BC20" s="36"/>
       <c r="BD20" s="25"/>
-      <c r="BE20" s="129">
+      <c r="BE20" s="118">
         <v>58</v>
       </c>
       <c r="BF20" s="28" t="str">
@@ -32618,7 +32618,7 @@
       </c>
       <c r="K21" s="70">
         <f>L21+M21+N21</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L21" s="70">
         <f>VLOOKUP(1,AA20:AK23,3,FALSE)</f>
@@ -32626,7 +32626,7 @@
       </c>
       <c r="M21" s="70">
         <f>VLOOKUP(1,AA20:AK23,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21" s="70">
         <f>VLOOKUP(1,AA20:AK23,5,FALSE)</f>
@@ -32638,7 +32638,7 @@
       </c>
       <c r="P21" s="71">
         <f>L21*3+M21</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R21" s="58">
         <f>DATE(2018,6,19)+TIME(4,0,0)+gmt_delta</f>
@@ -32674,7 +32674,7 @@
       </c>
       <c r="AA21" s="58">
         <f>COUNTIF(AN20:AN23,CONCATENATE("&gt;=",AN21))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB21" s="59" t="str">
         <f>VLOOKUP("Australia",T,lang,FALSE)</f>
@@ -32690,7 +32690,7 @@
       </c>
       <c r="AE21" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB21 &amp; "_lose")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF21" s="58">
         <f>SUMIF($E$7:$E$54,$AB21,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB21,$G$7:$G$54)</f>
@@ -32698,19 +32698,19 @@
       </c>
       <c r="AG21" s="58">
         <f>SUMIF($E$7:$E$54,$AB21,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB21,$F$7:$F$54)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AH21" s="58">
         <f>(AF21-AG21)*100+AK21*10000+AF21</f>
-        <v>9902</v>
+        <v>9702</v>
       </c>
       <c r="AI21" s="58">
         <f>AF21-AG21</f>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AJ21" s="58">
         <f>(AI21-AI25)/AI24</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AK21" s="58">
         <f>AC21*3+AD21</f>
@@ -32726,11 +32726,11 @@
       </c>
       <c r="AN21" s="59">
         <f>1000*AK21/AK24+100*AJ21+10*AF21/AF24+1*AL21/AL24+AM21</f>
-        <v>167.85751635714286</v>
+        <v>152.85751635714286</v>
       </c>
       <c r="AO21" s="60" t="str">
         <f>IF(SUM(AC20:AE23)=12,J22,INDEX(T,75,lang))</f>
-        <v>2C</v>
+        <v>Denmark</v>
       </c>
       <c r="AP21" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB21&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB21&amp;"_win")*($U$7:$U$54))</f>
@@ -32761,7 +32761,7 @@
       <c r="BB21" s="35"/>
       <c r="BC21" s="36"/>
       <c r="BD21" s="39"/>
-      <c r="BE21" s="130"/>
+      <c r="BE21" s="119"/>
       <c r="BF21" s="31" t="str">
         <f>T63</f>
         <v>W54</v>
@@ -32817,7 +32817,7 @@
       </c>
       <c r="K22" s="27">
         <f>L22+M22+N22</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L22" s="27">
         <f>VLOOKUP(2,AA20:AK23,3,FALSE)</f>
@@ -32825,7 +32825,7 @@
       </c>
       <c r="M22" s="27">
         <f>VLOOKUP(2,AA20:AK23,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N22" s="27">
         <f>VLOOKUP(2,AA20:AK23,5,FALSE)</f>
@@ -32837,7 +32837,7 @@
       </c>
       <c r="P22" s="73">
         <f>L22*3+M22</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R22" s="58">
         <f>DATE(2018,6,19)+TIME(1,0,0)+gmt_delta</f>
@@ -32873,7 +32873,7 @@
       </c>
       <c r="AA22" s="58">
         <f>COUNTIF(AN20:AN23,CONCATENATE("&gt;=",AN22))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB22" s="59" t="str">
         <f>VLOOKUP("Peru",T,lang,FALSE)</f>
@@ -32881,7 +32881,7 @@
       </c>
       <c r="AC22" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB22 &amp; "_win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD22" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB22 &amp; "_draw")</f>
@@ -32893,7 +32893,7 @@
       </c>
       <c r="AF22" s="58">
         <f>SUMIF($E$7:$E$54,$AB22,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB22,$G$7:$G$54)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG22" s="58">
         <f>SUMIF($E$7:$E$54,$AB22,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB22,$F$7:$F$54)</f>
@@ -32901,19 +32901,19 @@
       </c>
       <c r="AH22" s="58">
         <f>(AF22-AG22)*100+AK22*10000+AF22</f>
-        <v>-200</v>
+        <v>30002</v>
       </c>
       <c r="AI22" s="58">
         <f>AF22-AG22</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="AJ22" s="58">
         <f>(AI22-AI25)/AI24</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AK22" s="58">
         <f>AC22*3+AD22</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL22" s="58">
         <f>AP22/AP24*1000+AQ22/AQ24*100+AT22/AT24*10+AR22/AR24</f>
@@ -32925,7 +32925,7 @@
       </c>
       <c r="AN22" s="59">
         <f>1000*AK22/AK24+100*AJ22+10*AF22/AF24+1*AL22/AL24+AM22</f>
-        <v>5.6400000000000005E-4</v>
+        <v>488.57199257142855</v>
       </c>
       <c r="AP22" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB22&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB22&amp;"_win")*($U$7:$U$54))</f>
@@ -32947,7 +32947,7 @@
         <f>AR22-AS22</f>
         <v>0</v>
       </c>
-      <c r="AY22" s="129">
+      <c r="AY22" s="118">
         <v>54</v>
       </c>
       <c r="AZ22" s="28" t="str">
@@ -33010,31 +33010,31 @@
       </c>
       <c r="J23" s="72" t="str">
         <f>VLOOKUP(3,AA20:AK23,2,FALSE)</f>
-        <v>Australia</v>
+        <v>Peru</v>
       </c>
       <c r="K23" s="27">
         <f>L23+M23+N23</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L23" s="27">
         <f>VLOOKUP(3,AA20:AK23,3,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" s="27">
         <f>VLOOKUP(3,AA20:AK23,4,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23" s="27">
         <f>VLOOKUP(3,AA20:AK23,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O23" s="27" t="str">
         <f>VLOOKUP(3,AA20:AK23,6,FALSE) &amp; " - " &amp; VLOOKUP(3,AA20:AK23,7,FALSE)</f>
-        <v>2 - 3</v>
+        <v>2 - 2</v>
       </c>
       <c r="P23" s="73">
         <f>L23*3+M23</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R23" s="58">
         <f>DATE(2018,6,19)+TIME(7,0,0)+gmt_delta</f>
@@ -33082,7 +33082,7 @@
       </c>
       <c r="AD23" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB23 &amp; "_draw")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE23" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB23 &amp; "_lose")</f>
@@ -33098,7 +33098,7 @@
       </c>
       <c r="AH23" s="58">
         <f>(AF23-AG23)*100+AK23*10000+AF23</f>
-        <v>40102</v>
+        <v>50102</v>
       </c>
       <c r="AI23" s="58">
         <f>AF23-AG23</f>
@@ -33106,11 +33106,11 @@
       </c>
       <c r="AJ23" s="58">
         <f>(AI23-AI25)/AI24</f>
-        <v>0.6</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="AK23" s="58">
         <f>AC23*3+AD23</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL23" s="58">
         <f>AP23/AP24*1000+AQ23/AQ24*100+AT23/AT24*10+AR23/AR24</f>
@@ -33122,7 +33122,7 @@
       </c>
       <c r="AN23" s="59">
         <f>1000*AK23/AK24+100*AJ23+10*AF23/AF24+1*AL23/AL24+AM23</f>
-        <v>636.42912092857148</v>
+        <v>790.952930452381</v>
       </c>
       <c r="AP23" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB23&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB23&amp;"_win")*($U$7:$U$54))</f>
@@ -33144,7 +33144,7 @@
         <f>AR23-AS23</f>
         <v>0</v>
       </c>
-      <c r="AY23" s="130"/>
+      <c r="AY23" s="119"/>
       <c r="AZ23" s="31" t="str">
         <f>AO51</f>
         <v>2H</v>
@@ -33165,7 +33165,7 @@
       <c r="BN23" s="25"/>
       <c r="BO23" s="36"/>
       <c r="BP23" s="25"/>
-      <c r="BQ23" s="129">
+      <c r="BQ23" s="118">
         <v>64</v>
       </c>
       <c r="BR23" s="28" t="str">
@@ -33207,11 +33207,11 @@
       </c>
       <c r="J24" s="74" t="str">
         <f>VLOOKUP(4,AA20:AK23,2,FALSE)</f>
-        <v>Peru</v>
+        <v>Australia</v>
       </c>
       <c r="K24" s="75">
         <f>L24+M24+N24</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L24" s="75">
         <f>VLOOKUP(4,AA20:AK23,3,FALSE)</f>
@@ -33219,7 +33219,7 @@
       </c>
       <c r="M24" s="75">
         <f>VLOOKUP(4,AA20:AK23,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="75">
         <f>VLOOKUP(4,AA20:AK23,5,FALSE)</f>
@@ -33227,11 +33227,11 @@
       </c>
       <c r="O24" s="75" t="str">
         <f>VLOOKUP(4,AA20:AK23,6,FALSE) &amp; " - " &amp; VLOOKUP(4,AA20:AK23,7,FALSE)</f>
-        <v>0 - 2</v>
+        <v>2 - 5</v>
       </c>
       <c r="P24" s="76">
         <f>L24*3+M24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R24" s="58">
         <f>DATE(2018,6,20)+TIME(4,0,0)+gmt_delta</f>
@@ -33271,7 +33271,7 @@
       </c>
       <c r="AD24" s="58">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE24" s="58">
         <f t="shared" si="12"/>
@@ -33279,19 +33279,19 @@
       </c>
       <c r="AF24" s="58">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AG24" s="58">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AH24" s="58">
         <f>MAX(AH20:AH23)-AH25+1</f>
-        <v>60404</v>
+        <v>60502</v>
       </c>
       <c r="AI24" s="58">
         <f>MAX(AI20:AI23)-AI25+1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AK24" s="58">
         <f t="shared" si="12"/>
@@ -33338,7 +33338,7 @@
       <c r="BN24" s="25"/>
       <c r="BO24" s="36"/>
       <c r="BP24" s="39"/>
-      <c r="BQ24" s="130"/>
+      <c r="BQ24" s="119"/>
       <c r="BR24" s="31" t="str">
         <f>T77</f>
         <v>W62</v>
@@ -33417,11 +33417,11 @@
       </c>
       <c r="AH25" s="58">
         <f>MIN(AH20:AH23)</f>
-        <v>-200</v>
+        <v>9702</v>
       </c>
       <c r="AI25" s="58">
         <f>MIN(AI20:AI23)</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AY25" s="25" t="str">
         <f>INDEX(T,24+MONTH(R60),lang) &amp; " " &amp; DAY(R60) &amp; ", " &amp; YEAR(R60) &amp; "   " &amp; (IF(HOUR(R60)&lt;10,0,"")&amp;HOUR(R60)) &amp; ":" &amp;  (IF(MINUTE(R60)&lt;10,0,"")&amp;MINUTE(R60))</f>
@@ -33619,7 +33619,7 @@
         <f>AR26-AS26</f>
         <v>0</v>
       </c>
-      <c r="AY26" s="129">
+      <c r="AY26" s="118">
         <v>51</v>
       </c>
       <c r="AZ26" s="28" t="str">
@@ -33817,7 +33817,7 @@
         <f>AR27-AS27</f>
         <v>0</v>
       </c>
-      <c r="AY27" s="130"/>
+      <c r="AY27" s="119"/>
       <c r="AZ27" s="31" t="str">
         <f>AO9</f>
         <v>Russia</v>
@@ -34018,7 +34018,7 @@
       <c r="BB28" s="25"/>
       <c r="BC28" s="36"/>
       <c r="BD28" s="25"/>
-      <c r="BE28" s="129">
+      <c r="BE28" s="118">
         <v>59</v>
       </c>
       <c r="BF28" s="28" t="str">
@@ -34215,7 +34215,7 @@
       <c r="BB29" s="35"/>
       <c r="BC29" s="36"/>
       <c r="BD29" s="39"/>
-      <c r="BE29" s="130"/>
+      <c r="BE29" s="119"/>
       <c r="BF29" s="31" t="str">
         <f>T61</f>
         <v>W52</v>
@@ -34381,7 +34381,7 @@
         <f>MAX(AT26:AT29)-MIN(AT26:AT29)+1</f>
         <v>1</v>
       </c>
-      <c r="AY30" s="129">
+      <c r="AY30" s="118">
         <v>52</v>
       </c>
       <c r="AZ30" s="28" t="str">
@@ -34479,10 +34479,10 @@
         <f>MIN(AI26:AI29)</f>
         <v>-3</v>
       </c>
-      <c r="AY31" s="130"/>
+      <c r="AY31" s="119"/>
       <c r="AZ31" s="31" t="str">
         <f>AO21</f>
-        <v>2C</v>
+        <v>Denmark</v>
       </c>
       <c r="BA31" s="32"/>
       <c r="BB31" s="33"/>
@@ -34503,13 +34503,13 @@
       <c r="BN31" s="35"/>
       <c r="BO31" s="36"/>
       <c r="BP31" s="41"/>
-      <c r="BQ31" s="131" t="str">
+      <c r="BQ31" s="124" t="str">
         <f>INDEX(T,7,lang)</f>
         <v>Third-Place Play-Off</v>
       </c>
-      <c r="BR31" s="132"/>
-      <c r="BS31" s="132"/>
-      <c r="BT31" s="133"/>
+      <c r="BR31" s="125"/>
+      <c r="BS31" s="125"/>
+      <c r="BT31" s="126"/>
     </row>
     <row r="32" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18">
@@ -34693,7 +34693,7 @@
       <c r="BH32" s="25"/>
       <c r="BI32" s="36"/>
       <c r="BJ32" s="25"/>
-      <c r="BK32" s="129">
+      <c r="BK32" s="118">
         <v>62</v>
       </c>
       <c r="BL32" s="28" t="str">
@@ -34704,10 +34704,10 @@
       <c r="BN32" s="30"/>
       <c r="BO32" s="40"/>
       <c r="BP32" s="41"/>
-      <c r="BQ32" s="134"/>
-      <c r="BR32" s="135"/>
-      <c r="BS32" s="135"/>
-      <c r="BT32" s="136"/>
+      <c r="BQ32" s="127"/>
+      <c r="BR32" s="128"/>
+      <c r="BS32" s="128"/>
+      <c r="BT32" s="129"/>
     </row>
     <row r="33" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
@@ -34894,7 +34894,7 @@
       <c r="BH33" s="25"/>
       <c r="BI33" s="36"/>
       <c r="BJ33" s="39"/>
-      <c r="BK33" s="130"/>
+      <c r="BK33" s="119"/>
       <c r="BL33" s="31" t="str">
         <f>T72</f>
         <v>W60</v>
@@ -35074,7 +35074,7 @@
         <f>AR34-AS34</f>
         <v>0</v>
       </c>
-      <c r="AY34" s="129">
+      <c r="AY34" s="118">
         <v>55</v>
       </c>
       <c r="AZ34" s="28" t="str">
@@ -35271,7 +35271,7 @@
         <f>AR35-AS35</f>
         <v>0</v>
       </c>
-      <c r="AY35" s="130"/>
+      <c r="AY35" s="119"/>
       <c r="AZ35" s="31" t="str">
         <f>AO33</f>
         <v>2E</v>
@@ -35295,7 +35295,7 @@
       <c r="BN35" s="25"/>
       <c r="BO35" s="25"/>
       <c r="BP35" s="25"/>
-      <c r="BQ35" s="129">
+      <c r="BQ35" s="118">
         <v>63</v>
       </c>
       <c r="BR35" s="28" t="str">
@@ -35457,7 +35457,7 @@
       <c r="BB36" s="25"/>
       <c r="BC36" s="36"/>
       <c r="BD36" s="25"/>
-      <c r="BE36" s="129">
+      <c r="BE36" s="118">
         <v>60</v>
       </c>
       <c r="BF36" s="28" t="str">
@@ -35474,7 +35474,7 @@
       <c r="BN36" s="25"/>
       <c r="BO36" s="25"/>
       <c r="BP36" s="25"/>
-      <c r="BQ36" s="130"/>
+      <c r="BQ36" s="119"/>
       <c r="BR36" s="31" t="str">
         <f>Z77</f>
         <v>L62</v>
@@ -35561,7 +35561,7 @@
       <c r="BB37" s="35"/>
       <c r="BC37" s="36"/>
       <c r="BD37" s="39"/>
-      <c r="BE37" s="130"/>
+      <c r="BE37" s="119"/>
       <c r="BF37" s="31" t="str">
         <f>T65</f>
         <v>W56</v>
@@ -35751,7 +35751,7 @@
         <f>AR38-AS38</f>
         <v>1</v>
       </c>
-      <c r="AY38" s="129">
+      <c r="AY38" s="118">
         <v>56</v>
       </c>
       <c r="AZ38" s="28" t="str">
@@ -35945,7 +35945,7 @@
         <f>AR39-AS39</f>
         <v>0</v>
       </c>
-      <c r="AY39" s="130"/>
+      <c r="AY39" s="119"/>
       <c r="AZ39" s="31" t="str">
         <f>AO45</f>
         <v>2G</v>
@@ -36298,23 +36298,23 @@
         <f>AR41-AS41</f>
         <v>0</v>
       </c>
-      <c r="BJ41" s="146" t="str">
+      <c r="BJ41" s="120" t="str">
         <f>INDEX(T,102,lang)</f>
         <v>World Champion 2018</v>
       </c>
-      <c r="BK41" s="146"/>
-      <c r="BL41" s="146"/>
-      <c r="BM41" s="146"/>
-      <c r="BN41" s="146"/>
-      <c r="BO41" s="148" t="str">
+      <c r="BK41" s="120"/>
+      <c r="BL41" s="120"/>
+      <c r="BM41" s="120"/>
+      <c r="BN41" s="120"/>
+      <c r="BO41" s="122" t="str">
         <f>S85</f>
         <v/>
       </c>
-      <c r="BP41" s="148"/>
-      <c r="BQ41" s="148"/>
-      <c r="BR41" s="148"/>
-      <c r="BS41" s="148"/>
-      <c r="BT41" s="148"/>
+      <c r="BP41" s="122"/>
+      <c r="BQ41" s="122"/>
+      <c r="BR41" s="122"/>
+      <c r="BS41" s="122"/>
+      <c r="BT41" s="122"/>
     </row>
     <row r="42" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18">
@@ -36462,17 +36462,17 @@
         <f>MAX(AT38:AT41)-MIN(AT38:AT41)+1</f>
         <v>3</v>
       </c>
-      <c r="BJ42" s="147"/>
-      <c r="BK42" s="147"/>
-      <c r="BL42" s="147"/>
-      <c r="BM42" s="147"/>
-      <c r="BN42" s="147"/>
-      <c r="BO42" s="149"/>
-      <c r="BP42" s="149"/>
-      <c r="BQ42" s="149"/>
-      <c r="BR42" s="149"/>
-      <c r="BS42" s="149"/>
-      <c r="BT42" s="149"/>
+      <c r="BJ42" s="121"/>
+      <c r="BK42" s="121"/>
+      <c r="BL42" s="121"/>
+      <c r="BM42" s="121"/>
+      <c r="BN42" s="121"/>
+      <c r="BO42" s="123"/>
+      <c r="BP42" s="123"/>
+      <c r="BQ42" s="123"/>
+      <c r="BR42" s="123"/>
+      <c r="BS42" s="123"/>
+      <c r="BT42" s="123"/>
     </row>
     <row r="43" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18">
@@ -36494,8 +36494,12 @@
         <f>AB23</f>
         <v>Denmark</v>
       </c>
-      <c r="F43" s="23"/>
-      <c r="G43" s="24"/>
+      <c r="F43" s="23">
+        <v>0</v>
+      </c>
+      <c r="G43" s="24">
+        <v>0</v>
+      </c>
       <c r="H43" s="67" t="str">
         <f>AB20</f>
         <v>France</v>
@@ -36506,11 +36510,11 @@
       </c>
       <c r="S43" s="65" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Denmark_draw</v>
       </c>
       <c r="T43" s="65" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>France_draw</v>
       </c>
       <c r="U43" s="59">
         <f t="shared" si="4"/>
@@ -36528,9 +36532,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y43" s="58" t="str">
+      <c r="Y43" s="58">
         <f t="shared" si="9"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="AH43" s="58">
         <f>MIN(AH38:AH41)</f>
@@ -36562,8 +36566,12 @@
         <f>AB21</f>
         <v>Australia</v>
       </c>
-      <c r="F44" s="23"/>
-      <c r="G44" s="24"/>
+      <c r="F44" s="23">
+        <v>0</v>
+      </c>
+      <c r="G44" s="24">
+        <v>2</v>
+      </c>
       <c r="H44" s="67" t="str">
         <f>AB22</f>
         <v>Peru</v>
@@ -36602,11 +36610,11 @@
       </c>
       <c r="S44" s="65" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Australia_lose</v>
       </c>
       <c r="T44" s="65" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Peru_win</v>
       </c>
       <c r="U44" s="59">
         <f t="shared" si="4"/>
@@ -36624,9 +36632,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y44" s="58" t="str">
+      <c r="Y44" s="58">
         <f t="shared" si="9"/>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AA44" s="58">
         <f>COUNTIF(AN44:AN47,CONCATENATE("&gt;=",AN44))</f>
@@ -37038,12 +37046,12 @@
         <f>AR46-AS46</f>
         <v>0</v>
       </c>
-      <c r="AY46" s="137" t="s">
+      <c r="AY46" s="109" t="s">
         <v>2224</v>
       </c>
-      <c r="AZ46" s="138"/>
-      <c r="BA46" s="138"/>
-      <c r="BB46" s="139"/>
+      <c r="AZ46" s="110"/>
+      <c r="BA46" s="110"/>
+      <c r="BB46" s="111"/>
     </row>
     <row r="47" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18">
@@ -37207,10 +37215,10 @@
         <f>AR47-AS47</f>
         <v>0</v>
       </c>
-      <c r="AY47" s="140"/>
-      <c r="AZ47" s="141"/>
-      <c r="BA47" s="141"/>
-      <c r="BB47" s="142"/>
+      <c r="AY47" s="112"/>
+      <c r="AZ47" s="113"/>
+      <c r="BA47" s="113"/>
+      <c r="BB47" s="114"/>
     </row>
     <row r="48" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18">
@@ -37354,10 +37362,10 @@
         <f>MAX(AT44:AT47)-MIN(AT44:AT47)+1</f>
         <v>1</v>
       </c>
-      <c r="AY48" s="140"/>
-      <c r="AZ48" s="141"/>
-      <c r="BA48" s="141"/>
-      <c r="BB48" s="142"/>
+      <c r="AY48" s="112"/>
+      <c r="AZ48" s="113"/>
+      <c r="BA48" s="113"/>
+      <c r="BB48" s="114"/>
     </row>
     <row r="49" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18">
@@ -37425,10 +37433,10 @@
         <f>MIN(AI44:AI47)</f>
         <v>-8</v>
       </c>
-      <c r="AY49" s="140"/>
-      <c r="AZ49" s="141"/>
-      <c r="BA49" s="141"/>
-      <c r="BB49" s="142"/>
+      <c r="AY49" s="112"/>
+      <c r="AZ49" s="113"/>
+      <c r="BA49" s="113"/>
+      <c r="BB49" s="114"/>
     </row>
     <row r="50" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="18">
@@ -37596,10 +37604,10 @@
         <f>AR50-AS50</f>
         <v>0</v>
       </c>
-      <c r="AY50" s="140"/>
-      <c r="AZ50" s="141"/>
-      <c r="BA50" s="141"/>
-      <c r="BB50" s="142"/>
+      <c r="AY50" s="112"/>
+      <c r="AZ50" s="113"/>
+      <c r="BA50" s="113"/>
+      <c r="BB50" s="114"/>
     </row>
     <row r="51" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="18">
@@ -37767,10 +37775,10 @@
         <f>AR51-AS51</f>
         <v>0</v>
       </c>
-      <c r="AY51" s="140"/>
-      <c r="AZ51" s="141"/>
-      <c r="BA51" s="141"/>
-      <c r="BB51" s="142"/>
+      <c r="AY51" s="112"/>
+      <c r="AZ51" s="113"/>
+      <c r="BA51" s="113"/>
+      <c r="BB51" s="114"/>
     </row>
     <row r="52" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18">
@@ -37934,10 +37942,10 @@
         <f>AR52-AS52</f>
         <v>0</v>
       </c>
-      <c r="AY52" s="143"/>
-      <c r="AZ52" s="144"/>
-      <c r="BA52" s="144"/>
-      <c r="BB52" s="145"/>
+      <c r="AY52" s="115"/>
+      <c r="AZ52" s="116"/>
+      <c r="BA52" s="116"/>
+      <c r="BB52" s="117"/>
     </row>
     <row r="53" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18">
@@ -38526,6 +38534,27 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="hexNDhodxxdoIYhe+LOVPFyB2v0aJLQphXCm5lZGwHDaP2ZITl3Lpck5mriyKWgCt8wrzYbwlizwv7dyeeElyw==" saltValue="swcCixFXOL0FnpwQehLBng==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="28">
+    <mergeCell ref="BQ6:BT7"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="A5:H6"/>
+    <mergeCell ref="J5:P6"/>
+    <mergeCell ref="AY10:AY11"/>
+    <mergeCell ref="BE12:BE13"/>
+    <mergeCell ref="AY6:BB7"/>
+    <mergeCell ref="BE6:BH7"/>
+    <mergeCell ref="BK6:BN7"/>
+    <mergeCell ref="AY22:AY23"/>
+    <mergeCell ref="BQ23:BQ24"/>
+    <mergeCell ref="AY18:AY19"/>
+    <mergeCell ref="BE20:BE21"/>
+    <mergeCell ref="AY14:AY15"/>
+    <mergeCell ref="BK16:BK17"/>
+    <mergeCell ref="AY30:AY31"/>
+    <mergeCell ref="BQ31:BT32"/>
+    <mergeCell ref="BK32:BK33"/>
+    <mergeCell ref="AY26:AY27"/>
+    <mergeCell ref="BE28:BE29"/>
     <mergeCell ref="AY46:BB52"/>
     <mergeCell ref="AY38:AY39"/>
     <mergeCell ref="BJ41:BN42"/>
@@ -38533,27 +38562,6 @@
     <mergeCell ref="BQ35:BQ36"/>
     <mergeCell ref="BE36:BE37"/>
     <mergeCell ref="BO41:BT42"/>
-    <mergeCell ref="AY30:AY31"/>
-    <mergeCell ref="BQ31:BT32"/>
-    <mergeCell ref="BK32:BK33"/>
-    <mergeCell ref="AY26:AY27"/>
-    <mergeCell ref="BE28:BE29"/>
-    <mergeCell ref="AY22:AY23"/>
-    <mergeCell ref="BQ23:BQ24"/>
-    <mergeCell ref="AY18:AY19"/>
-    <mergeCell ref="BE20:BE21"/>
-    <mergeCell ref="AY14:AY15"/>
-    <mergeCell ref="BK16:BK17"/>
-    <mergeCell ref="AY10:AY11"/>
-    <mergeCell ref="BE12:BE13"/>
-    <mergeCell ref="AY6:BB7"/>
-    <mergeCell ref="BE6:BH7"/>
-    <mergeCell ref="BK6:BN7"/>
-    <mergeCell ref="BQ6:BT7"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="A5:H6"/>
-    <mergeCell ref="J5:P6"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="F7:F55">

</xml_diff>

<commit_message>
Update the last game scores in group stage and the template
</commit_message>
<xml_diff>
--- a/input/world_cup_2018_final.xlsx
+++ b/input/world_cup_2018_final.xlsx
@@ -29896,8 +29896,8 @@
   </sheetPr>
   <dimension ref="A1:BT97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -32952,7 +32952,7 @@
       </c>
       <c r="AZ22" s="28" t="str">
         <f>AO44</f>
-        <v>1G</v>
+        <v>Belgium</v>
       </c>
       <c r="BA22" s="29"/>
       <c r="BB22" s="30"/>
@@ -33147,7 +33147,7 @@
       <c r="AY23" s="130"/>
       <c r="AZ23" s="31" t="str">
         <f>AO51</f>
-        <v>2H</v>
+        <v>Senegal</v>
       </c>
       <c r="BA23" s="32"/>
       <c r="BB23" s="33"/>
@@ -35756,7 +35756,7 @@
       </c>
       <c r="AZ38" s="28" t="str">
         <f>AO50</f>
-        <v>1H</v>
+        <v>Colombia</v>
       </c>
       <c r="BA38" s="29"/>
       <c r="BB38" s="30"/>
@@ -35948,7 +35948,7 @@
       <c r="AY39" s="130"/>
       <c r="AZ39" s="31" t="str">
         <f>AO45</f>
-        <v>2G</v>
+        <v>England</v>
       </c>
       <c r="BA39" s="32"/>
       <c r="BB39" s="33"/>
@@ -36646,7 +36646,7 @@
       </c>
       <c r="AC44" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB44 &amp; "_win")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD44" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB44 &amp; "_draw")</f>
@@ -36658,7 +36658,7 @@
       </c>
       <c r="AF44" s="58">
         <f>SUMIF($E$7:$E$54,$AB44,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB44,$G$7:$G$54)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AG44" s="58">
         <f>SUMIF($E$7:$E$54,$AB44,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB44,$F$7:$F$54)</f>
@@ -36666,19 +36666,19 @@
       </c>
       <c r="AH44" s="58">
         <f>(AF44-AG44)*100+AK44*10000+AF44</f>
-        <v>60608</v>
+        <v>90709</v>
       </c>
       <c r="AI44" s="58">
         <f>AF44-AG44</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AJ44" s="58">
         <f>(AI44-AI49)/AI48</f>
-        <v>0.93333333333333335</v>
+        <v>0.94117647058823528</v>
       </c>
       <c r="AK44" s="58">
         <f>AC44*3+AD44</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AL44" s="58">
         <f>AP44/AP48*1000+AQ44/AQ48*100+AT44/AT48*10+AR44/AR48</f>
@@ -36690,11 +36690,11 @@
       </c>
       <c r="AN44" s="59">
         <f>1000*AK44/AK48+100*AJ44+10*AF44/AF48+1*AL44/AL48+AM44</f>
-        <v>960.47685297619046</v>
+        <v>1005.3683095588235</v>
       </c>
       <c r="AO44" s="60" t="str">
         <f>IF(SUM(AC44:AE47)=12,J45,INDEX(T,82,lang))</f>
-        <v>1G</v>
+        <v>Belgium</v>
       </c>
       <c r="AP44" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB44&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB44&amp;"_win")*($U$7:$U$54))</f>
@@ -36753,11 +36753,11 @@
       </c>
       <c r="K45" s="70">
         <f>L45+M45+N45</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L45" s="70">
         <f>VLOOKUP(1,AA44:AK47,3,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M45" s="70">
         <f>VLOOKUP(1,AA44:AK47,4,FALSE)</f>
@@ -36769,11 +36769,11 @@
       </c>
       <c r="O45" s="70" t="str">
         <f>VLOOKUP(1,AA44:AK47,6,FALSE) &amp; " - " &amp; VLOOKUP(1,AA44:AK47,7,FALSE)</f>
-        <v>8 - 2</v>
+        <v>9 - 2</v>
       </c>
       <c r="P45" s="71">
         <f>L45*3+M45</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="R45" s="58">
         <f>DATE(2018,6,26)+TIME(7,0,0)+gmt_delta</f>
@@ -36825,23 +36825,23 @@
       </c>
       <c r="AE45" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB45 &amp; "_lose")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF45" s="58">
         <f>SUMIF($E$7:$E$54,$AB45,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB45,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG45" s="58">
         <f>SUMIF($E$7:$E$54,$AB45,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB45,$F$7:$F$54)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AH45" s="58">
         <f>(AF45-AG45)*100+AK45*10000+AF45</f>
-        <v>-799</v>
+        <v>-898</v>
       </c>
       <c r="AI45" s="58">
         <f>AF45-AG45</f>
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="AJ45" s="58">
         <f>(AI45-AI49)/AI48</f>
@@ -36861,11 +36861,11 @@
       </c>
       <c r="AN45" s="59">
         <f>1000*AK45/AK48+100*AJ45+10*AF45/AF48+1*AL45/AL48+AM45</f>
-        <v>1.2503105000000001</v>
+        <v>2.5003104999999999</v>
       </c>
       <c r="AO45" s="60" t="str">
         <f>IF(SUM(AC44:AE47)=12,J46,INDEX(T,83,lang))</f>
-        <v>2G</v>
+        <v>England</v>
       </c>
       <c r="AP45" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB45&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB45&amp;"_win")*($U$7:$U$54))</f>
@@ -36924,7 +36924,7 @@
       </c>
       <c r="K46" s="27">
         <f>L46+M46+N46</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L46" s="27">
         <f>VLOOKUP(2,AA44:AK47,3,FALSE)</f>
@@ -36936,11 +36936,11 @@
       </c>
       <c r="N46" s="27">
         <f>VLOOKUP(2,AA44:AK47,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O46" s="27" t="str">
         <f>VLOOKUP(2,AA44:AK47,6,FALSE) &amp; " - " &amp; VLOOKUP(2,AA44:AK47,7,FALSE)</f>
-        <v>8 - 2</v>
+        <v>8 - 3</v>
       </c>
       <c r="P46" s="73">
         <f>L46*3+M46</f>
@@ -36988,7 +36988,7 @@
       </c>
       <c r="AC46" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB46 &amp; "_win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD46" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB46 &amp; "_draw")</f>
@@ -37000,27 +37000,27 @@
       </c>
       <c r="AF46" s="58">
         <f>SUMIF($E$7:$E$54,$AB46,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB46,$G$7:$G$54)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AG46" s="58">
         <f>SUMIF($E$7:$E$54,$AB46,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB46,$F$7:$F$54)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AH46" s="58">
         <f>(AF46-AG46)*100+AK46*10000+AF46</f>
-        <v>-397</v>
+        <v>29705</v>
       </c>
       <c r="AI46" s="58">
         <f>AF46-AG46</f>
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="AJ46" s="58">
         <f>(AI46-AI49)/AI48</f>
-        <v>0.26666666666666666</v>
+        <v>0.35294117647058826</v>
       </c>
       <c r="AK46" s="58">
         <f>AC46*3+AD46</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL46" s="58">
         <f>AP46/AP48*1000+AQ46/AQ48*100+AT46/AT48*10+AR46/AR48</f>
@@ -37032,7 +37032,7 @@
       </c>
       <c r="AN46" s="59">
         <f>1000*AK46/AK48+100*AJ46+10*AF46/AF48+1*AL46/AL48+AM46</f>
-        <v>30.417085666666669</v>
+        <v>341.54453664705886</v>
       </c>
       <c r="AP46" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB46&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB46&amp;"_win")*($U$7:$U$54))</f>
@@ -37097,11 +37097,11 @@
       </c>
       <c r="K47" s="27">
         <f>L47+M47+N47</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L47" s="27">
         <f>VLOOKUP(3,AA44:AK47,3,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M47" s="27">
         <f>VLOOKUP(3,AA44:AK47,4,FALSE)</f>
@@ -37113,11 +37113,11 @@
       </c>
       <c r="O47" s="27" t="str">
         <f>VLOOKUP(3,AA44:AK47,6,FALSE) &amp; " - " &amp; VLOOKUP(3,AA44:AK47,7,FALSE)</f>
-        <v>3 - 7</v>
+        <v>5 - 8</v>
       </c>
       <c r="P47" s="73">
         <f>L47*3+M47</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R47" s="58">
         <f>DATE(2018,6,27)+TIME(7,0,0)+gmt_delta</f>
@@ -37169,7 +37169,7 @@
       </c>
       <c r="AE47" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB47 &amp; "_lose")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF47" s="58">
         <f>SUMIF($E$7:$E$54,$AB47,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB47,$G$7:$G$54)</f>
@@ -37177,19 +37177,19 @@
       </c>
       <c r="AG47" s="58">
         <f>SUMIF($E$7:$E$54,$AB47,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB47,$F$7:$F$54)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH47" s="58">
         <f>(AF47-AG47)*100+AK47*10000+AF47</f>
-        <v>60608</v>
+        <v>60508</v>
       </c>
       <c r="AI47" s="58">
         <f>AF47-AG47</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AJ47" s="58">
         <f>(AI47-AI49)/AI48</f>
-        <v>0.93333333333333335</v>
+        <v>0.82352941176470584</v>
       </c>
       <c r="AK47" s="58">
         <f>AC47*3+AD47</f>
@@ -37205,7 +37205,7 @@
       </c>
       <c r="AN47" s="59">
         <f>1000*AK47/AK48+100*AJ47+10*AF47/AF48+1*AL47/AL48+AM47</f>
-        <v>960.47671397619047</v>
+        <v>692.35346467647059</v>
       </c>
       <c r="AP47" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB47&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB47&amp;"_win")*($U$7:$U$54))</f>
@@ -37268,7 +37268,7 @@
       </c>
       <c r="K48" s="75">
         <f>L48+M48+N48</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L48" s="75">
         <f>VLOOKUP(4,AA44:AK47,3,FALSE)</f>
@@ -37280,11 +37280,11 @@
       </c>
       <c r="N48" s="75">
         <f>VLOOKUP(4,AA44:AK47,5,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O48" s="75" t="str">
         <f>VLOOKUP(4,AA44:AK47,6,FALSE) &amp; " - " &amp; VLOOKUP(4,AA44:AK47,7,FALSE)</f>
-        <v>1 - 9</v>
+        <v>2 - 11</v>
       </c>
       <c r="P48" s="76">
         <f>L48*3+M48</f>
@@ -37324,7 +37324,7 @@
       </c>
       <c r="AC48" s="58">
         <f t="shared" ref="AC48:AL48" si="16">MAX(AC44:AC47)-MIN(AC44:AC47)+1</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AD48" s="58">
         <f t="shared" si="16"/>
@@ -37332,7 +37332,7 @@
       </c>
       <c r="AE48" s="58">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AF48" s="58">
         <f t="shared" si="16"/>
@@ -37340,19 +37340,19 @@
       </c>
       <c r="AG48" s="58">
         <f t="shared" si="16"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AH48" s="58">
         <f>MAX(AH44:AH47)-AH49+1</f>
-        <v>61408</v>
+        <v>91608</v>
       </c>
       <c r="AI48" s="58">
         <f>MAX(AI44:AI47)-AI49+1</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AK48" s="58">
         <f t="shared" si="16"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AL48" s="58">
         <f t="shared" si="16"/>
@@ -37447,11 +37447,11 @@
       </c>
       <c r="AH49" s="58">
         <f>MIN(AH44:AH47)</f>
-        <v>-799</v>
+        <v>-898</v>
       </c>
       <c r="AI49" s="58">
         <f>MIN(AI44:AI47)</f>
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="AY49" s="140"/>
       <c r="AZ49" s="141"/>
@@ -37558,7 +37558,7 @@
       </c>
       <c r="AC50" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB50 &amp; "_win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD50" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB50 &amp; "_draw")</f>
@@ -37570,7 +37570,7 @@
       </c>
       <c r="AF50" s="58">
         <f>SUMIF($E$7:$E$54,$AB50,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB50,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG50" s="58">
         <f>SUMIF($E$7:$E$54,$AB50,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB50,$F$7:$F$54)</f>
@@ -37578,11 +37578,11 @@
       </c>
       <c r="AH50" s="58">
         <f>(AF50-AG50)*100+AK50*10000+AF50</f>
-        <v>-399</v>
+        <v>29702</v>
       </c>
       <c r="AI50" s="58">
         <f>AF50-AG50</f>
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="AJ50" s="58">
         <f>(AI50-AI55)/AI54</f>
@@ -37590,7 +37590,7 @@
       </c>
       <c r="AK50" s="58">
         <f>AC50*3+AD50</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL50" s="58">
         <f>AP50/AP54*1000+AQ50/AQ54*100+AT50/AT54*10+AR50/AR54</f>
@@ -37602,11 +37602,11 @@
       </c>
       <c r="AN50" s="59">
         <f>1000*AK50/AK54+100*AJ50+10*AF50/AF54+1*AL50/AL54+AM50</f>
-        <v>2.5006045000000001</v>
+        <v>755.00060450000001</v>
       </c>
       <c r="AO50" s="60" t="str">
         <f>IF(SUM(AC50:AE53)=12,J51,INDEX(T,84,lang))</f>
-        <v>1H</v>
+        <v>Colombia</v>
       </c>
       <c r="AP50" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB50&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB50&amp;"_win")*($U$7:$U$54))</f>
@@ -37653,39 +37653,43 @@
         <f>AB47</f>
         <v>England</v>
       </c>
-      <c r="F51" s="23"/>
-      <c r="G51" s="24"/>
+      <c r="F51" s="23">
+        <v>0</v>
+      </c>
+      <c r="G51" s="24">
+        <v>1</v>
+      </c>
       <c r="H51" s="67" t="str">
         <f>AB44</f>
         <v>Belgium</v>
       </c>
       <c r="J51" s="69" t="str">
         <f>VLOOKUP(1,AA50:AK53,2,FALSE)</f>
-        <v>Senegal</v>
+        <v>Colombia</v>
       </c>
       <c r="K51" s="70">
         <f>L51+M51+N51</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L51" s="70">
         <f>VLOOKUP(1,AA50:AK53,3,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M51" s="70">
         <f>VLOOKUP(1,AA50:AK53,4,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N51" s="70">
         <f>VLOOKUP(1,AA50:AK53,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O51" s="70" t="str">
         <f>VLOOKUP(1,AA50:AK53,6,FALSE) &amp; " - " &amp; VLOOKUP(1,AA50:AK53,7,FALSE)</f>
-        <v>4 - 3</v>
+        <v>5 - 2</v>
       </c>
       <c r="P51" s="71">
         <f>L51*3+M51</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R51" s="58">
         <f>DATE(2018,6,28)+TIME(7,0,0)+gmt_delta</f>
@@ -37693,11 +37697,11 @@
       </c>
       <c r="S51" s="65" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>England_lose</v>
       </c>
       <c r="T51" s="65" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Belgium_win</v>
       </c>
       <c r="U51" s="59">
         <f t="shared" si="4"/>
@@ -37715,13 +37719,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y51" s="58" t="str">
+      <c r="Y51" s="58">
         <f t="shared" si="9"/>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AA51" s="58">
         <f>COUNTIF(AN50:AN53,CONCATENATE("&gt;=",AN51))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB51" s="59" t="str">
         <f>VLOOKUP("Senegal",T,lang,FALSE)</f>
@@ -37737,7 +37741,7 @@
       </c>
       <c r="AE51" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB51 &amp; "_lose")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF51" s="58">
         <f>SUMIF($E$7:$E$54,$AB51,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB51,$G$7:$G$54)</f>
@@ -37745,19 +37749,19 @@
       </c>
       <c r="AG51" s="58">
         <f>SUMIF($E$7:$E$54,$AB51,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB51,$F$7:$F$54)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH51" s="58">
         <f>(AF51-AG51)*100+AK51*10000+AF51</f>
-        <v>40104</v>
+        <v>40004</v>
       </c>
       <c r="AI51" s="58">
         <f>AF51-AG51</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ51" s="58">
         <f>(AI51-AI55)/AI54</f>
-        <v>0.7142857142857143</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="AK51" s="58">
         <f>AC51*3+AD51</f>
@@ -37773,11 +37777,11 @@
       </c>
       <c r="AN51" s="59">
         <f>1000*AK51/AK54+100*AJ51+10*AF51/AF54+1*AL51/AL54+AM51</f>
-        <v>882.40965858986181</v>
+        <v>1053.8382300184333</v>
       </c>
       <c r="AO51" s="60" t="str">
         <f>IF(SUM(AC50:AE53)=12,J52,INDEX(T,85,lang))</f>
-        <v>2H</v>
+        <v>Senegal</v>
       </c>
       <c r="AP51" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB51&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB51&amp;"_win")*($U$7:$U$54))</f>
@@ -37824,19 +37828,23 @@
         <f>AB45</f>
         <v>Panama</v>
       </c>
-      <c r="F52" s="23"/>
-      <c r="G52" s="24"/>
+      <c r="F52" s="23">
+        <v>1</v>
+      </c>
+      <c r="G52" s="24">
+        <v>2</v>
+      </c>
       <c r="H52" s="67" t="str">
         <f>AB46</f>
         <v>Tunisia</v>
       </c>
       <c r="J52" s="72" t="str">
         <f>VLOOKUP(2,AA50:AK53,2,FALSE)</f>
-        <v>Japan</v>
+        <v>Senegal</v>
       </c>
       <c r="K52" s="27">
         <f>L52+M52+N52</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L52" s="27">
         <f>VLOOKUP(2,AA50:AK53,3,FALSE)</f>
@@ -37848,11 +37856,11 @@
       </c>
       <c r="N52" s="27">
         <f>VLOOKUP(2,AA50:AK53,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O52" s="27" t="str">
         <f>VLOOKUP(2,AA50:AK53,6,FALSE) &amp; " - " &amp; VLOOKUP(2,AA50:AK53,7,FALSE)</f>
-        <v>4 - 3</v>
+        <v>4 - 4</v>
       </c>
       <c r="P52" s="73">
         <f>L52*3+M52</f>
@@ -37864,11 +37872,11 @@
       </c>
       <c r="S52" s="65" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Panama_lose</v>
       </c>
       <c r="T52" s="65" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Tunisia_win</v>
       </c>
       <c r="U52" s="59">
         <f t="shared" si="4"/>
@@ -37886,13 +37894,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y52" s="58" t="str">
+      <c r="Y52" s="58">
         <f t="shared" si="9"/>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AA52" s="58">
         <f>COUNTIF(AN50:AN53,CONCATENATE("&gt;=",AN52))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB52" s="59" t="str">
         <f>VLOOKUP("Colombia",T,lang,FALSE)</f>
@@ -37900,7 +37908,7 @@
       </c>
       <c r="AC52" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB52 &amp; "_win")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD52" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB52 &amp; "_draw")</f>
@@ -37912,7 +37920,7 @@
       </c>
       <c r="AF52" s="58">
         <f>SUMIF($E$7:$E$54,$AB52,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB52,$G$7:$G$54)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG52" s="58">
         <f>SUMIF($E$7:$E$54,$AB52,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB52,$F$7:$F$54)</f>
@@ -37920,11 +37928,11 @@
       </c>
       <c r="AH52" s="58">
         <f>(AF52-AG52)*100+AK52*10000+AF52</f>
-        <v>30204</v>
+        <v>60305</v>
       </c>
       <c r="AI52" s="58">
         <f>AF52-AG52</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ52" s="58">
         <f>(AI52-AI55)/AI54</f>
@@ -37932,7 +37940,7 @@
       </c>
       <c r="AK52" s="58">
         <f>AC52*3+AD52</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AL52" s="58">
         <f>AP52/AP54*1000+AQ52/AQ54*100+AT52/AT54*10+AR52/AR54</f>
@@ -37944,7 +37952,7 @@
       </c>
       <c r="AN52" s="59">
         <f>1000*AK52/AK54+100*AJ52+10*AF52/AF54+1*AL52/AL54+AM52</f>
-        <v>695.71482471428567</v>
+        <v>1598.2148247142857</v>
       </c>
       <c r="AP52" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB52&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB52&amp;"_win")*($U$7:$U$54))</f>
@@ -37991,19 +37999,23 @@
         <f>AB53</f>
         <v>Japan</v>
       </c>
-      <c r="F53" s="23"/>
-      <c r="G53" s="24"/>
+      <c r="F53" s="23">
+        <v>0</v>
+      </c>
+      <c r="G53" s="24">
+        <v>1</v>
+      </c>
       <c r="H53" s="67" t="str">
         <f>AB50</f>
         <v>Poland</v>
       </c>
       <c r="J53" s="72" t="str">
         <f>VLOOKUP(3,AA50:AK53,2,FALSE)</f>
-        <v>Colombia</v>
+        <v>Japan</v>
       </c>
       <c r="K53" s="27">
         <f>L53+M53+N53</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L53" s="27">
         <f>VLOOKUP(3,AA50:AK53,3,FALSE)</f>
@@ -38011,7 +38023,7 @@
       </c>
       <c r="M53" s="27">
         <f>VLOOKUP(3,AA50:AK53,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N53" s="27">
         <f>VLOOKUP(3,AA50:AK53,5,FALSE)</f>
@@ -38019,11 +38031,11 @@
       </c>
       <c r="O53" s="27" t="str">
         <f>VLOOKUP(3,AA50:AK53,6,FALSE) &amp; " - " &amp; VLOOKUP(3,AA50:AK53,7,FALSE)</f>
-        <v>4 - 2</v>
+        <v>4 - 4</v>
       </c>
       <c r="P53" s="73">
         <f>L53*3+M53</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R53" s="58">
         <f>DATE(2018,6,28)+TIME(3,0,0)+gmt_delta</f>
@@ -38031,11 +38043,11 @@
       </c>
       <c r="S53" s="65" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Japan_lose</v>
       </c>
       <c r="T53" s="65" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Poland_win</v>
       </c>
       <c r="U53" s="59">
         <f t="shared" si="4"/>
@@ -38053,13 +38065,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y53" s="58" t="str">
+      <c r="Y53" s="58">
         <f t="shared" si="9"/>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AA53" s="58">
         <f>COUNTIF(AN50:AN53,CONCATENATE("&gt;=",AN53))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB53" s="59" t="str">
         <f>VLOOKUP("Japan",T,lang,FALSE)</f>
@@ -38075,7 +38087,7 @@
       </c>
       <c r="AE53" s="58">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB53 &amp; "_lose")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF53" s="58">
         <f>SUMIF($E$7:$E$54,$AB53,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB53,$G$7:$G$54)</f>
@@ -38083,19 +38095,19 @@
       </c>
       <c r="AG53" s="58">
         <f>SUMIF($E$7:$E$54,$AB53,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB53,$F$7:$F$54)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH53" s="58">
         <f>(AF53-AG53)*100+AK53*10000+AF53</f>
-        <v>40104</v>
+        <v>40004</v>
       </c>
       <c r="AI53" s="58">
         <f>AF53-AG53</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ53" s="58">
         <f>(AI53-AI55)/AI54</f>
-        <v>0.7142857142857143</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="AK53" s="58">
         <f>AC53*3+AD53</f>
@@ -38111,7 +38123,7 @@
       </c>
       <c r="AN53" s="59">
         <f>1000*AK53/AK54+100*AJ53+10*AF53/AF54+1*AL53/AL54+AM53</f>
-        <v>882.40951658986182</v>
+        <v>1053.8380880184332</v>
       </c>
       <c r="AP53" s="61">
         <f>SUMPRODUCT(($S$7:$S$54=AB53&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB53&amp;"_win")*($U$7:$U$54))</f>
@@ -38154,8 +38166,12 @@
         <f>AB51</f>
         <v>Senegal</v>
       </c>
-      <c r="F54" s="32"/>
-      <c r="G54" s="33"/>
+      <c r="F54" s="32">
+        <v>0</v>
+      </c>
+      <c r="G54" s="33">
+        <v>1</v>
+      </c>
       <c r="H54" s="68" t="str">
         <f>AB52</f>
         <v>Colombia</v>
@@ -38166,11 +38182,11 @@
       </c>
       <c r="K54" s="75">
         <f>L54+M54+N54</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L54" s="75">
         <f>VLOOKUP(4,AA50:AK53,3,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M54" s="75">
         <f>VLOOKUP(4,AA50:AK53,4,FALSE)</f>
@@ -38182,11 +38198,11 @@
       </c>
       <c r="O54" s="75" t="str">
         <f>VLOOKUP(4,AA50:AK53,6,FALSE) &amp; " - " &amp; VLOOKUP(4,AA50:AK53,7,FALSE)</f>
-        <v>1 - 5</v>
+        <v>2 - 5</v>
       </c>
       <c r="P54" s="76">
         <f>L54*3+M54</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R54" s="58">
         <f>DATE(2018,6,28)+TIME(3,0,0)+gmt_delta</f>
@@ -38194,11 +38210,11 @@
       </c>
       <c r="S54" s="65" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Senegal_lose</v>
       </c>
       <c r="T54" s="65" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Colombia_win</v>
       </c>
       <c r="U54" s="59">
         <f t="shared" si="4"/>
@@ -38216,9 +38232,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y54" s="58" t="str">
+      <c r="Y54" s="58">
         <f t="shared" si="9"/>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AC54" s="58">
         <f t="shared" ref="AC54:AL54" si="17">MAX(AC50:AC53)-MIN(AC50:AC53)+1</f>
@@ -38230,7 +38246,7 @@
       </c>
       <c r="AE54" s="58">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF54" s="58">
         <f t="shared" si="17"/>
@@ -38242,7 +38258,7 @@
       </c>
       <c r="AH54" s="58">
         <f>MAX(AH50:AH53)-AH55+1</f>
-        <v>40504</v>
+        <v>30604</v>
       </c>
       <c r="AI54" s="58">
         <f>MAX(AI50:AI53)-AI55+1</f>
@@ -38250,7 +38266,7 @@
       </c>
       <c r="AK54" s="58">
         <f t="shared" si="17"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AL54" s="58">
         <f t="shared" si="17"/>
@@ -38296,11 +38312,11 @@
       <c r="P55" s="49"/>
       <c r="AH55" s="58">
         <f>MIN(AH50:AH53)</f>
-        <v>-399</v>
+        <v>29702</v>
       </c>
       <c r="AI55" s="58">
         <f>MIN(AI50:AI53)</f>
-        <v>-4</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="56" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>